<commit_message>
Modificaciones en TC de CREDIN Nueva semilla ConfirmadebitoCVU Nueva test suite DEBIN (Sprint36) Nueva accion ConfirmadebitoCVU"
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - CREDIN - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - CREDIN - Escenarios y Casos de Pruebas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A61100E-024B-49A3-A267-11418E4F7DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAF0C12-BBF4-4DC3-A62A-F8C6404FBBD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Credin" sheetId="7" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Credin!$A$1:$E$107</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Credin!$A$1:$E$108</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="242">
   <si>
     <t>Parametros</t>
   </si>
@@ -312,9 +312,6 @@
     <t>"objeto":{"tipo":"TRANSFERENCIA"},"umbral_riesgo":100,"debito":{"cuit":"20000000222","banco":"001","sucursal":"0207","cuenta":{"cbu":"0000207500000000000055"},"titular":"string"},"credito":{"cuit":"27348075093","banco":"086","sucursal":"0010","cuenta":{"cbu":"0860010302800023724781"},"titular":"string"},"concepto":"VAR","idUsuario":11231,"idComprobante":9228098,"importe":{"moneda":"032","importe":2950},"mismoTitular":0,"ori_trx":"","ori_terminal":"","ori_adicional":"","datosGenerador":{"ipCliente":"","tipoDispositivo":"","plataforma":"","imsi":"","imei":"","ubicacion":{"lat":0,"lng":0,"precision":0}},"descripcion":"Descripcion"</t>
   </si>
   <si>
-    <t>"objeto":{"tipo":"TRANSFERENCIA"},"umbral_riesgo":100,"debito":{"cuit":"20000000222","banco":"000","sucursal":"0208","cuenta":{"cbu":"0000207500000000000055"},"titular":"string"},"credito":{"cuit":"27348075093","banco":"086","sucursal":"0010","cuenta":{"cbu":"0860010302800023724781"},"titular":"string"},"concepto":"VAR","idUsuario":11231,"idComprobante":9228098,"importe":{"moneda":"032","importe":2950},"mismoTitular":0,"ori_trx":"","ori_terminal":"","ori_adicional":"","datosGenerador":{"ipCliente":"","tipoDispositivo":"","plataforma":"","imsi":"","imei":"","ubicacion":{"lat":0,"lng":0,"precision":0}},"descripcion":"Descripcion"</t>
-  </si>
-  <si>
     <t>"objeto":{"tipo":"TRANSFERENCIA"},"umbral_riesgo":100,"debito":{"cuit":"20000000222","banco":"000","sucursal":"0207","cuenta":{"cbu":"000020750000000000005"},"titular":"string"},"credito":{"cuit":"27348075093","banco":"086","sucursal":"0010","cuenta":{"cbu":"0860010302800023724781"},"titular":"string"},"concepto":"VAR","idUsuario":11231,"idComprobante":9228098,"importe":{"moneda":"032","importe":2950},"mismoTitular":0,"ori_trx":"","ori_terminal":"","ori_adicional":"","datosGenerador":{"ipCliente":"","tipoDispositivo":"","plataforma":"","imsi":"","imei":"","ubicacion":{"lat":0,"lng":0,"precision":0}},"descripcion":"Descripcion"</t>
   </si>
   <si>
@@ -342,9 +339,6 @@
     <t>"objeto":{"tipo":"TRANSFERENCIA"},"umbral_riesgo":100,"debito":{"cuit":"20000000222","banco":"BANCO000","sucursal":"0207","cuenta":{"cbu":"0000207500000000000055"},"titular":"string"},"credito":{"cuit":"20263275064","banco":"000","sucursal":"0097","cuenta":{"cbu":"0000097000000000000116"},"titular":"string"},"concepto":"VAR","idUsuario":11231,"idComprobante":9228098,"importe":{"moneda":"032","importe":2950},"mismoTitular":0,"ori_trx":"","ori_terminal":"","ori_adicional":"","datosGenerador":{"ipCliente":"","tipoDispositivo":"","plataforma":"","imsi":"","imei":"","ubicacion":{"lat":0,"lng":0,"precision":0}},"descripcion":"Descripcion"</t>
   </si>
   <si>
-    <t>"objeto":{"tipo":"TRANSFERENCIA"},"umbral_riesgo":100,"debito":{"cuit":"20000000222","banco":"000","sucursal":"0SUC 207","cuenta":{"cbu":"0000207500000000000055"},"titular":"string"},"credito":{"cuit":"20263275064","banco":"000","sucursal":"0097","cuenta":{"cbu":"0000097000000000000116"},"titular":"string"},"concepto":"VAR","idUsuario":11231,"idComprobante":9228098,"importe":{"moneda":"032","importe":2950},"mismoTitular":0,"ori_trx":"","ori_terminal":"","ori_adicional":"","datosGenerador":{"ipCliente":"","tipoDispositivo":"","plataforma":"","imsi":"","imei":"","ubicacion":{"lat":0,"lng":0,"precision":0}},"descripcion":"Descripcion"</t>
-  </si>
-  <si>
     <t>"objeto":{"tipo":"TRANSFERENCIA"},"umbral_riesgo":100,"debito":{"cuit":"20959558790","banco":"000","sucursal":"0207","cuenta":{"cbu":"0000207500000000000055"},"titular":"string"},"credito":{"cuit":"20263275064","banco":"000","sucursal":"0097","cuenta":{"cbu":"0000097000000000000116"},"titular":"string"},"concepto":"VAR","idUsuario":11231,"idComprobante":9228098,"importe":{"moneda":"032","importe":2950},"mismoTitular":0,"ori_trx":"","ori_terminal":"","ori_adicional":"","datosGenerador":{"ipCliente":"","tipoDispositivo":"","plataforma":"","imsi":"","imei":"","ubicacion":{"lat":0,"lng":0,"precision":0}},"descripcion":"Descripcion"</t>
   </si>
   <si>
@@ -576,22 +570,6 @@
     <t>{"StatusCode":200,"Mensaje":{"respuesta": {"codigo":"01","descripcion":"NO EXISTE EL CBU VENDEDOR"}}}</t>
   </si>
   <si>
-    <t>{"StatusCode":200,"Mensaje":{"respuesta": {"codigo":"99","descripcion":"BANCO VENDEDOR NO HABILITADO PARA TRANSACCIONES"}}}</t>
-  </si>
-  <si>
-    <t>{"StatusCode":200,"Mensaje":{"respuesta": {"codigo":"08","descripcion":"ERROR CUENTA VIRTUAL DEL COMPRADOR"}}}</t>
-  </si>
-  <si>
-    <t>{"StatusCode":200,"Mensaje":{"respuesta": {"codigo":"99","descripcion":"BANCO COMPRADOR NO HABILITADO PARA TRANSACCIONES"}}}</t>
-  </si>
-  <si>
-    <t>{"StatusCode":200,"Mensaje":{"respuesta":{"codigo":"99","descripcion":"BANCO COMPRADOR NO HABILITADO PARA TRANSACCIONES"}}}</t>
-  </si>
-  <si>
-    <t>{"StatusCode":200,"Mensaje":{"respuesta": {"codigo": "09",
-        "descripcion": "CUENTA MAL FORMULADO DEL COMPRADOR"}}}</t>
-  </si>
-  <si>
     <t>"objeto":{"tipo":"TRANSFERENCIA"},"umbral_riesgo":100,"debito":{"cuit":"20000009998","banco":"998","sucursal":"0547","cuenta":{"cbu":"998054740000000000005"},"titular":"string"},"credito":{"cuit":"20263275064","banco":"000","sucursal":"0097","cuenta":{"cbu":"0000097000000000000116"},"titular":"string"},"concepto":"VAR","idUsuario":11231,"idComprobante":9228098,"importe":{"moneda":"032","importe":2950},"mismoTitular":0,"ori_trx":"","ori_terminal":"","ori_adicional":"","datosGenerador":{"ipCliente":"","tipoDispositivo":"","plataforma":"","imsi":"","imei":"","ubicacion":{"lat":0,"lng":0,"precision":0}},"descripcion":"Descripcion"</t>
   </si>
   <si>
@@ -679,18 +657,12 @@
     <t>"objeto":{"tipo":"TRANSFERENCIA"},"umbral_riesgo":100,"debito":{"cuit":"20000009998","banco":"998","sucursal":"0547","cuenta":{"cbu":"9980547400000000000055"},"titular":"string"},"credito":{"cuit":"2795955879","banco":"415","sucursal":"0999","cuenta":{"cbu":"4150999718001586640025"},"titular":"string"},"concepto":"VAR","idUsuario":11231,"idComprobante":9228098,"importe":{"moneda":"032","importe":6000},"mismoTitular":0,"ori_trx":"","ori_terminal":"","ori_adicional":"","datosGenerador":{"ipCliente":"","tipoDispositivo":"","plataforma":"","imsi":"","imei":"","ubicacion":{"lat":0,"lng":0,"precision":0}},"descripcion":"Descripcion"</t>
   </si>
   <si>
-    <t xml:space="preserve">{"StatusCode":200,"Mensaje":{"respuesta": {"codigo":"01","descripcion":"NO EXISTE EL CBU VENDEDOR"}}} </t>
-  </si>
-  <si>
     <t>Credin - Ingresar  banco vendedor Inexistente o Erroneo - CBU-CBU</t>
   </si>
   <si>
     <t>"objeto":{"tipo":"TRANSFERENCIA"},"umbral_riesgo":100,"debito":{"cuit":"20000009998","banco":"998","sucursal":"0547","cuenta":{"cbu":"9980547400000000000055"},"titular":"string"},"credito":{"cuit":"23076812179","banco":"415","sucursal":"0999","cuenta":{"cbu":"4150999718001586640123"},"titular":"string"},"concepto":"VAR","idUsuario":11231,"idComprobante":9228098,"importe":{"moneda":"032","importe":6000},"mismoTitular":0,"ori_trx":"","ori_terminal":"","ori_adicional":"","datosGenerador":{"ipCliente":"","tipoDispositivo":"","plataforma":"","imsi":"","imei":"","ubicacion":{"lat":0,"lng":0,"precision":0}},"descripcion":"Descripcion"</t>
   </si>
   <si>
-    <t>{"StatusCode":200,"Mensaje":{"respuesta": {"codigo":"09","descripcion":"CUENTA MAL FORMULADO DEL VENDEDOR"}}}</t>
-  </si>
-  <si>
     <t>Credin - Ingresar CBU vendedor inexistente CBU-CBU</t>
   </si>
   <si>
@@ -718,15 +690,6 @@
     <t xml:space="preserve">{"StatusCode":200,"Mensaje":{"respuesta":{"codigo":"99","descripcion":"BANCO VENDEDOR NO HABILITADO PARA TRANSACCIONES"}}} </t>
   </si>
   <si>
-    <t xml:space="preserve">{"StatusCode":200,"Mensaje":{"respuesta": {"codigo":"99","descripcion":"BANCO VENDEDOR NO HABILITADO PARA TRANSACCIONES"}}} </t>
-  </si>
-  <si>
-    <t>{"StatusCode":200,"Mensaje":{"respuesta": {"codigo":"08","descripcion":"ERROR CUENTA VIRTUAL DEL VENDEDOR"}}</t>
-  </si>
-  <si>
-    <t>{"StatusCode":200,"Mensaje":{"respuesta": {"codigo":"08","descripcion":"ERROR CUENTA VIRTUAL DEL VENDEDOR"}}}</t>
-  </si>
-  <si>
     <t>Credin - Ingresar  banco vendedor Inexistente o Erroneo - CVU-CVU</t>
   </si>
   <si>
@@ -736,9 +699,6 @@
     <t>"objeto":{"tipo":"TRANSFERENCIA"},"umbral_riesgo":100,"debito":{"cuit":"20000000222","banco":"000","sucursal":"0207","cuenta":{"cbu":"0000207500000000000055"},"titular":"string"},"credito":{"cuit":"20263275064","banco":"000","sucursal":"0097","cuenta":{"cbu":"0000097000000000000123"},"titular":"string"},"concepto":"VAR","idUsuario":11231,"idComprobante":9228098,"importe":{"moneda":"032","importe":2950},"mismoTitular":0,"ori_trx":"","ori_terminal":"","ori_adicional":"","datosGenerador":{"ipCliente":"","tipoDispositivo":"","plataforma":"","imsi":"","imei":"","ubicacion":{"lat":0,"lng":0,"precision":0}},"descripcion":"Descripcion"</t>
   </si>
   <si>
-    <t>{"StatusCode":200,"Mensaje":{"respuesta": {"codigo":"01","descripcion":"NO EXISTE EL CBU VENDEDOR"}}</t>
-  </si>
-  <si>
     <t>"objeto":{"tipo":"TRANSFERENCIA"},"umbral_riesgo":100,"debito":{"cuit":"20000009998","banco":"998","sucursal":"0547","cuenta":{"cbu":"9980547400000000000055"},"titular":"string"},"credito":{"cuit":"27959558790","banco":"000","sucursal":"0097","cuenta":{"cbu":"0000097000000000000116"},"titular":"string"},"concepto":"VAR","idUsuario":11231,"idComprobante":9228098,"importe":{"moneda":"032","importe":2950},"mismoTitular":0,"ori_trx":"","ori_terminal":"","ori_adicional":"","datosGenerador":{"ipCliente":"","tipoDispositivo":"","plataforma":"","imsi":"","imei":"","ubicacion":{"lat":0,"lng":0,"precision":0}},"descripcion":"Descripcion"</t>
   </si>
   <si>
@@ -767,13 +727,46 @@
   </si>
   <si>
     <t>"objeto":{"tipo":"TRANSFERENCIA"},"umbral_riesgo":100,"debito":{"cuit":"20000000222","banco":"000","sucursal":"0207","cuenta":{"cbu":"0000207500000000000055"},"titular":"string"},"credito":{"cuit":"27348075093","banco":"01000","sucursal":"0010","cuenta":{"cbu":"0860010302800023724781"},"titular":"string"},"concepto":"VAR","idUsuario":11231,"idComprobante":9228098,"importe":{"moneda":"032","importe":2950},"mismoTitular":0,"ori_trx":"","ori_terminal":"","ori_adicional":"","datosGenerador":{"ipCliente":"","tipoDispositivo":"","plataforma":"","imsi":"","imei":"","ubicacion":{"lat":0,"lng":0,"precision":0}},"descripcion":"Descripcion"</t>
+  </si>
+  <si>
+    <t>"objeto":{"tipo":"TRANSFERENCIA"},"umbral_riesgo":100,"debito":{"cuit":"20000000222","banco":"000","sucursal":"0207","cuenta":{"cbu":"0000207500000000000055"},"titular":"string"},"credito":{"cuit":"27348075093","banco":"086","sucursal":"0010","cuenta":{"cbu":"0860010302800023724781"},"titular":"string"},"concepto":"FCE","idUsuario":11231,"idComprobante":9228098,"importe":{"moneda":"032","importe":2950},"mismoTitular":0,"ori_trx":"","ori_terminal":"","ori_adicional":"","datosGenerador":{"ipCliente":"","tipoDispositivo":"","plataforma":"","imsi":"","imei":"","ubicacion":{"lat":0,"lng":0,"precision":0}},"descripcion":"Descripcion"</t>
+  </si>
+  <si>
+    <t>Credin - CONCEPTO FCE</t>
+  </si>
+  <si>
+    <t>{"StatusCode":200,"Mensaje":{"respuesta": {"codigo":"10","descripcion":"CUIT MAL FORMULADO DEL COMPRADOR"}}}</t>
+  </si>
+  <si>
+    <t>{"StatusCode":200,"Mensaje":{"respuesta": {"codigo":"09","descripcion":"BANCO MAL FORMULADO DEL COMPRADOR"}}}</t>
+  </si>
+  <si>
+    <t>{"StatusCode":200,"Mensaje":{"respuesta": {"codigo":"09","descripcion":"CUIT MAL FORMULADO DEL VENDEDOR"}}}</t>
+  </si>
+  <si>
+    <t>{"StatusCode":200,"Mensaje":{"respuesta": {"codigo":"09","descripcion":"BANCO MAL FORMULADO DEL VENDEDOR"}}}</t>
+  </si>
+  <si>
+    <t>{"StatusCode":200,"Mensaje":{"respuesta": {"codigo":"24","descripcion":"CBU MAL FORMULADO DEL COMPRADOR"}}}</t>
+  </si>
+  <si>
+    <t>{"StatusCode":200,"Mensaje":{"respuesta": {"codigo":"23","descripcion":"CBU MAL FORMULADO DEL VENDEDOR"}}}</t>
+  </si>
+  <si>
+    <t>{"respuesta":{"codigo":"99","descripcion":"BANCO VENDEDOR NO HABILITADO PARA TRANSACCIONES"}</t>
+  </si>
+  <si>
+    <t>"objeto":{"tipo":"TRANSFERENCIA"},"umbral_riesgo":100,"debito":{"cuit":"20000000222","banco":"000","sucursal":"020888","cuenta":{"cbu":"0000207500000000000055"},"titular":"string"},"credito":{"cuit":"27348075093","banco":"086","sucursal":"0010","cuenta":{"cbu":"0860010302800023724781"},"titular":"string"},"concepto":"VAR","idUsuario":11231,"idComprobante":9228098,"importe":{"moneda":"032","importe":2950},"mismoTitular":0,"ori_trx":"","ori_terminal":"","ori_adicional":"","datosGenerador":{"ipCliente":"","tipoDispositivo":"","plataforma":"","imsi":"","imei":"","ubicacion":{"lat":0,"lng":0,"precision":0}},"descripcion":"Descripcion"</t>
+  </si>
+  <si>
+    <t>"objeto":{"tipo":"TRANSFERENCIA"},"umbral_riesgo":100,"debito":{"cuit":"20000000222","banco":"000","sucursal":"SUC 207","cuenta":{"cbu":"0000207500000000000055"},"titular":"string"},"credito":{"cuit":"20263275064","banco":"000","sucursal":"0097","cuenta":{"cbu":"0000097000000000000116"},"titular":"string"},"concepto":"VAR","idUsuario":11231,"idComprobante":9228098,"importe":{"moneda":"032","importe":2950},"mismoTitular":0,"ori_trx":"","ori_terminal":"","ori_adicional":"","datosGenerador":{"ipCliente":"","tipoDispositivo":"","plataforma":"","imsi":"","imei":"","ubicacion":{"lat":0,"lng":0,"precision":0}},"descripcion":"Descripcion"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -781,13 +774,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -802,7 +813,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -826,21 +837,23 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
+          <fgColor rgb="FFFFFF00"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -848,7 +861,15 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1129,10 +1150,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63218BCB-F1F0-4D18-A551-3DB8181D382F}">
-  <dimension ref="A1:E107"/>
+  <dimension ref="A1:E108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,7 +1191,7 @@
         <v>76</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>64</v>
@@ -1187,7 +1208,7 @@
         <v>76</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>65</v>
@@ -1206,8 +1227,8 @@
       <c r="C4" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>67</v>
+      <c r="D4" s="11" t="s">
+        <v>233</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>7</v>
@@ -1223,8 +1244,8 @@
       <c r="C5" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>183</v>
+      <c r="D5" s="11" t="s">
+        <v>234</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>9</v>
@@ -1243,7 +1264,7 @@
       <c r="D6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="13" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1255,10 +1276,10 @@
         <v>76</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>67</v>
+        <v>169</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>237</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>12</v>
@@ -1274,8 +1295,8 @@
       <c r="C8" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>179</v>
+      <c r="D8" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>25</v>
@@ -1291,8 +1312,8 @@
       <c r="C9" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>180</v>
+      <c r="D9" s="11" t="s">
+        <v>236</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>26</v>
@@ -1306,7 +1327,7 @@
         <v>76</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>68</v>
@@ -1325,8 +1346,8 @@
       <c r="C11" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>179</v>
+      <c r="D11" s="11" t="s">
+        <v>237</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>28</v>
@@ -1340,13 +1361,13 @@
         <v>76</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>69</v>
       </c>
       <c r="E12" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -1357,7 +1378,7 @@
         <v>76</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>70</v>
@@ -1374,7 +1395,7 @@
         <v>76</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>64</v>
@@ -1391,13 +1412,13 @@
         <v>76</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E15" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -1408,13 +1429,13 @@
         <v>76</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E16" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -1425,13 +1446,13 @@
         <v>76</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E17" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -1442,13 +1463,13 @@
         <v>76</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E18" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -1459,13 +1480,13 @@
         <v>76</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E19" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -1476,13 +1497,13 @@
         <v>76</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E20" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -1493,13 +1514,13 @@
         <v>76</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E21" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -1510,13 +1531,13 @@
         <v>76</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E22" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="23" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -1527,13 +1548,13 @@
         <v>76</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E23" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -1544,13 +1565,13 @@
         <v>76</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E24" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -1561,1407 +1582,1424 @@
         <v>76</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E25" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>56329</v>
+        <v>57403</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>143</v>
+        <v>231</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E26" t="s">
-        <v>197</v>
+        <v>232</v>
       </c>
     </row>
     <row r="27" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
-        <v>56330</v>
+        <v>56329</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E27" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="28" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
-        <v>56331</v>
+        <v>56330</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E28" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>56332</v>
+        <v>56331</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E29" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="30" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
-        <v>56333</v>
+        <v>56332</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>212</v>
+        <v>144</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E30" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
-        <v>56334</v>
+        <v>56333</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>147</v>
+        <v>205</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E31" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="32" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
-        <v>56335</v>
+        <v>56334</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E32" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
-        <v>56336</v>
+        <v>56335</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E33" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="34" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
-        <v>56337</v>
+        <v>56336</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E34" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="35" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
-        <v>56338</v>
+        <v>56337</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E35" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="36" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
-        <v>56339</v>
+        <v>56338</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E36" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
-        <v>56340</v>
+        <v>56339</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>131</v>
+        <v>150</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E37" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
+        <v>56340</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
         <v>56341</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E38" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
-        <v>56342</v>
-      </c>
       <c r="B39" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>69</v>
       </c>
       <c r="E39" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A40" s="6">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>56342</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E40" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
         <v>56061</v>
       </c>
-      <c r="B40" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E40" s="6" t="s">
+      <c r="B41" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>56124</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E41" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A42">
+        <v>56124</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>56175</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D42" s="2" t="s">
+      <c r="B43" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E42" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A43" s="6">
+      <c r="E43" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
         <v>56126</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C43" s="8" t="s">
+      <c r="B44" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D44" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E43" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A44" s="6">
-        <v>56127</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>184</v>
-      </c>
       <c r="E44" s="6" t="s">
-        <v>13</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
-        <v>56378</v>
-      </c>
-      <c r="B45" s="9" t="s">
+        <v>56127</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>214</v>
+        <v>84</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>237</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
+        <v>56378</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A47" s="6">
         <v>56379</v>
       </c>
-      <c r="B46" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C46" s="8" t="s">
+      <c r="B47" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D46" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="D47" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A48">
         <v>56416</v>
       </c>
-      <c r="B47" t="s">
-        <v>76</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D47" s="2" t="s">
+      <c r="B48" t="s">
+        <v>76</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E48" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A48" s="6">
+    <row r="49" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A49" s="6">
         <v>56417</v>
       </c>
-      <c r="B48" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C48" s="8" t="s">
+      <c r="B49" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D48" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="E48" s="6" t="s">
+      <c r="D49" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="E49" s="6" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A49" s="9">
-        <v>56476</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A50" s="9">
+        <v>56476</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A51" s="9">
         <v>56477</v>
       </c>
-      <c r="B50" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="D50" s="7" t="s">
+      <c r="B51" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D51" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E50" s="6" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A51" s="6">
-        <v>56158</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>181</v>
-      </c>
       <c r="E51" s="6" t="s">
-        <v>18</v>
+        <v>214</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
+        <v>56158</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A53" s="6">
         <v>56159</v>
       </c>
-      <c r="B52" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C52" s="8" t="s">
+      <c r="B53" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C53" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="E52" s="6" t="s">
+      <c r="D53" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="E53" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A53" s="6">
+    <row r="54" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A54" s="6">
         <v>56160</v>
       </c>
-      <c r="B53" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C53" s="8" t="s">
+      <c r="B54" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C54" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D53" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="E53" s="6" t="s">
+      <c r="D54" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E54" s="6" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A54" s="6">
-        <v>56161</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
-        <v>56162</v>
+        <v>56161</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>181</v>
+        <v>90</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>233</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
+        <v>56162</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A57" s="6">
         <v>56163</v>
       </c>
-      <c r="B56" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A57" s="6">
+      <c r="B57" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A58" s="6">
         <v>56181</v>
       </c>
-      <c r="B57" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C57" s="8" t="s">
+      <c r="B58" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D58" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="D57" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A58" s="6">
-        <v>56164</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>67</v>
-      </c>
       <c r="E58" s="6" t="s">
-        <v>23</v>
+        <v>170</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
-        <v>56165</v>
+        <v>56164</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>67</v>
+        <v>237</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
+        <v>56165</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A61" s="6">
         <v>56457</v>
       </c>
-      <c r="B60" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A61" s="6">
+      <c r="B61" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A62" s="6">
         <v>56461</v>
       </c>
-      <c r="B61" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C61" s="8" t="s">
+      <c r="B62" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A63" s="6">
+        <v>56462</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C63" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D61" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A62" s="6">
-        <v>56462</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="E62" s="6" t="s">
+      <c r="D63" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="E63" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A63" s="6">
+    <row r="64" spans="1:5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A64" s="6">
         <v>56463</v>
       </c>
-      <c r="B63" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="D63" s="2" t="s">
+      <c r="B64" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D64" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E64" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A64" s="6">
-        <v>56464</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D64" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="E64" s="6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A65" s="6">
-        <v>56465</v>
+        <v>56464</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="D65" s="7" t="s">
-        <v>179</v>
+        <v>96</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>238</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
+        <v>56465</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="D66" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A67" s="6">
         <v>56466</v>
       </c>
-      <c r="B66" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C66" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="D66" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="E66" s="6" t="s">
+      <c r="B67" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="E67" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="67" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A67" s="6">
+    <row r="68" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A68" s="6">
         <v>56469</v>
       </c>
-      <c r="B67" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="D67" s="2" t="s">
+      <c r="B68" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E68" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A68" s="6">
-        <v>56467</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="E68" s="10" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A69" s="6">
-        <v>56468</v>
+        <v>56467</v>
       </c>
       <c r="B69" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="D69" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>219</v>
+        <v>98</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="E69" s="10" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A70" s="6">
-        <v>56170</v>
+        <v>56468</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>100</v>
+        <v>211</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>38</v>
+        <v>210</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A71" s="6">
+        <v>56170</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A72" s="6">
         <v>56171</v>
       </c>
-      <c r="B71" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C71" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="E71" s="6" t="s">
+      <c r="B72" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D72" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="E72" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A72" s="6">
+    <row r="73" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A73" s="6">
         <v>56172</v>
       </c>
-      <c r="B72" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D72" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="E72" s="6" t="s">
+      <c r="B73" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="D73" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E73" s="6" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A73" s="6">
-        <v>56173</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C73" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="D73" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A74" s="6">
-        <v>56174</v>
+        <v>56173</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>181</v>
+        <v>101</v>
+      </c>
+      <c r="D74" s="11" t="s">
+        <v>233</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
-        <v>56125</v>
+        <v>56174</v>
       </c>
       <c r="B75" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="D75" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="E75" s="10" t="s">
-        <v>169</v>
+        <v>102</v>
+      </c>
+      <c r="D75" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A76" s="6">
-        <v>56182</v>
+        <v>56125</v>
       </c>
       <c r="B76" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="D76" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>174</v>
+        <v>103</v>
+      </c>
+      <c r="D76" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A77" s="6">
-        <v>56176</v>
+        <v>56182</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>106</v>
+        <v>174</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>43</v>
+        <v>172</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A78" s="6">
+        <v>56176</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D78" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A79" s="6">
         <v>56177</v>
       </c>
-      <c r="B78" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D78" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E78" s="6" t="s">
+      <c r="B79" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D79" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="E79" s="6" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A79" s="6">
-        <v>56478</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C79" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D79" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A80" s="6">
-        <v>56479</v>
+        <v>56478</v>
       </c>
       <c r="B80" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="D80" s="12" t="s">
-        <v>229</v>
+        <v>106</v>
+      </c>
+      <c r="D80" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A81" s="6">
+        <v>56479</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D81" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A82" s="6">
         <v>56480</v>
       </c>
-      <c r="B81" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="D81" s="12" t="s">
-        <v>229</v>
-      </c>
-      <c r="E81" s="6" t="s">
+      <c r="B82" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D82" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E82" s="6" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A82" s="6">
-        <v>56482</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="D82" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="E82" s="6" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A83" s="6">
-        <v>56481</v>
+        <v>56482</v>
       </c>
       <c r="B83" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="D83" s="7" t="s">
-        <v>229</v>
+        <v>109</v>
+      </c>
+      <c r="D83" s="11" t="s">
+        <v>238</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A84" s="6">
-        <v>56492</v>
+        <v>56481</v>
       </c>
       <c r="B84" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D84" s="12" t="s">
-        <v>229</v>
+        <v>110</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>230</v>
+        <v>48</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A85" s="6">
-        <v>56493</v>
+        <v>56492</v>
       </c>
       <c r="B85" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="D85" s="12" t="s">
-        <v>229</v>
+        <v>111</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>239</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A86" s="6">
-        <v>56496</v>
+        <v>56493</v>
       </c>
       <c r="B86" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="D86" s="7" t="s">
-        <v>179</v>
+        <v>112</v>
+      </c>
+      <c r="D86" s="14" t="s">
+        <v>73</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>49</v>
+        <v>219</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A87" s="6">
+        <v>56496</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D87" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A88" s="6">
         <v>56186</v>
       </c>
-      <c r="B87" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C87" s="8" t="s">
+      <c r="B88" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D88" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="E88" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A89" s="6">
+        <v>56187</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D89" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="E89" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A90" s="6">
+        <v>56188</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E90" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A91" s="6">
+        <v>56189</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C91" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="D87" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E87" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A88" s="6">
-        <v>56187</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C88" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="D88" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="E88" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A89" s="6">
-        <v>56188</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C89" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="D89" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E89" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A90" s="6">
-        <v>56189</v>
-      </c>
-      <c r="B90" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C90" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D90" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E90" s="6" t="s">
+      <c r="D91" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="E91" s="6" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A91" s="6">
-        <v>56190</v>
-      </c>
-      <c r="B91" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C91" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="D91" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E91" s="6" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="92" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A92" s="6">
+        <v>56190</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E92" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A93" s="6">
         <v>56191</v>
       </c>
-      <c r="B92" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C92" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="D92" s="7" t="s">
+      <c r="B93" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D93" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E92" s="6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A93" s="6">
-        <v>56192</v>
-      </c>
-      <c r="B93" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C93" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="D93" s="7" t="s">
-        <v>67</v>
-      </c>
       <c r="E93" s="6" t="s">
-        <v>55</v>
+        <v>166</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A94" s="6">
-        <v>56193</v>
+        <v>56192</v>
       </c>
       <c r="B94" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="D94" s="7" t="s">
-        <v>67</v>
+        <v>178</v>
+      </c>
+      <c r="D94" s="11" t="s">
+        <v>237</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A95" s="6">
+        <v>56193</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D95" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="E95" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A96" s="6">
         <v>56498</v>
       </c>
-      <c r="B95" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C95" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="D95" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="E95" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A96" s="6">
-        <v>56499</v>
-      </c>
       <c r="B96" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>120</v>
+        <v>220</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>229</v>
+        <v>177</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>58</v>
+        <v>215</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A97" s="6">
-        <v>56500</v>
+        <v>56499</v>
       </c>
       <c r="B97" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="D97" s="7" t="s">
-        <v>229</v>
+        <v>118</v>
+      </c>
+      <c r="D97" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A98" s="6">
+        <v>56500</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D98" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="E98" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A99" s="6">
         <v>56501</v>
       </c>
-      <c r="B98" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C98" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="D98" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="E98" s="6" t="s">
+      <c r="B99" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D99" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E99" s="6" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A99" s="6">
-        <v>56503</v>
-      </c>
-      <c r="B99" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C99" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="D99" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E99" s="6" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A100" s="6">
-        <v>56506</v>
+        <v>56503</v>
       </c>
       <c r="B100" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="D100" s="7" t="s">
-        <v>229</v>
+        <v>121</v>
+      </c>
+      <c r="D100" s="11" t="s">
+        <v>238</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A101" s="6">
-        <v>56519</v>
+        <v>56506</v>
       </c>
       <c r="B101" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="D101" s="7" t="s">
-        <v>229</v>
+        <v>221</v>
+      </c>
+      <c r="D101" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>235</v>
+        <v>62</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A102" s="6">
-        <v>56520</v>
+        <v>56519</v>
       </c>
       <c r="B102" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="D102" s="7" t="s">
-        <v>229</v>
+        <v>122</v>
+      </c>
+      <c r="D102" s="14" t="s">
+        <v>239</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A103" s="6">
+        <v>56520</v>
+      </c>
+      <c r="B103" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D103" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E103" s="6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A104" s="6">
         <v>56522</v>
       </c>
-      <c r="B103" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C103" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="D103" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="E103" s="6" t="s">
+      <c r="B104" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C104" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D104" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="E104" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="104" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A104" s="6">
+    <row r="105" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A105" s="6">
         <v>56194</v>
       </c>
-      <c r="B104" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C104" s="8" t="s">
+      <c r="B105" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C105" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E105" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A106" s="6">
+        <v>56523</v>
+      </c>
+      <c r="B106" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C106" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D106" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D104" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="E104" s="6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A105" s="6">
-        <v>56523</v>
-      </c>
-      <c r="B105" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C105" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="D105" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="E105" s="6" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A106">
-        <v>56664</v>
-      </c>
-      <c r="B106" t="s">
-        <v>76</v>
-      </c>
-      <c r="C106" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="E106" t="s">
-        <v>238</v>
+      <c r="E106" s="6" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="107" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A107">
+        <v>56664</v>
+      </c>
+      <c r="B107" t="s">
+        <v>76</v>
+      </c>
+      <c r="C107" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E107" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A108">
         <v>56665</v>
       </c>
-      <c r="B107" t="s">
-        <v>76</v>
-      </c>
-      <c r="C107" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="E107" t="s">
-        <v>239</v>
+      <c r="B108" t="s">
+        <v>76</v>
+      </c>
+      <c r="C108" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E108" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
debin error ori_trx_id TC Garantia, modificaciones CREDIN TC debin
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - CREDIN - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - CREDIN - Escenarios y Casos de Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAF0C12-BBF4-4DC3-A62A-F8C6404FBBD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79AA4C1-E4C6-44DA-AAD4-97F8B2C467E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="241">
   <si>
     <t>Parametros</t>
   </si>
@@ -751,9 +751,6 @@
   </si>
   <si>
     <t>{"StatusCode":200,"Mensaje":{"respuesta": {"codigo":"23","descripcion":"CBU MAL FORMULADO DEL VENDEDOR"}}}</t>
-  </si>
-  <si>
-    <t>{"respuesta":{"codigo":"99","descripcion":"BANCO VENDEDOR NO HABILITADO PARA TRANSACCIONES"}</t>
   </si>
   <si>
     <t>"objeto":{"tipo":"TRANSFERENCIA"},"umbral_riesgo":100,"debito":{"cuit":"20000000222","banco":"000","sucursal":"020888","cuenta":{"cbu":"0000207500000000000055"},"titular":"string"},"credito":{"cuit":"27348075093","banco":"086","sucursal":"0010","cuenta":{"cbu":"0860010302800023724781"},"titular":"string"},"concepto":"VAR","idUsuario":11231,"idComprobante":9228098,"importe":{"moneda":"032","importe":2950},"mismoTitular":0,"ori_trx":"","ori_terminal":"","ori_adicional":"","datosGenerador":{"ipCliente":"","tipoDispositivo":"","plataforma":"","imsi":"","imei":"","ubicacion":{"lat":0,"lng":0,"precision":0}},"descripcion":"Descripcion"</t>
@@ -781,24 +778,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -813,21 +798,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -837,35 +809,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1152,1853 +1109,1853 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63218BCB-F1F0-4D18-A551-3DB8181D382F}">
   <dimension ref="A1:E108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="88.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="53.85546875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="89.7109375" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="6"/>
+    <col min="1" max="1" width="14.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="88.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="53.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="89.7109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>53628</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+    <row r="3" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>53629</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="4">
         <v>53630</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="B4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="4">
         <v>53631</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="B5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+    <row r="6" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>53632</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>77</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="4">
         <v>53633</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C7" s="8" t="s">
+      <c r="B7" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="4">
         <v>53634</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="8" t="s">
+      <c r="B8" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="4">
         <v>53635</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" s="8" t="s">
+      <c r="B9" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+    <row r="10" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
         <v>53636</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="B10" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>127</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="A11" s="4">
         <v>53637</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="8" t="s">
+      <c r="B11" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+    <row r="12" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <v>53638</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>128</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="13" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+    <row r="13" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>53639</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="B13" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>227</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+    <row r="14" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>53640</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="B14" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>129</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+    <row r="15" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>53431</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="B15" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>130</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="16" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+    <row r="16" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
         <v>53432</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="B16" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>131</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="17" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+    <row r="17" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
         <v>53433</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="B17" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>132</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="18" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+    <row r="18" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
         <v>53434</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="B18" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>133</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="19" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+    <row r="19" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
         <v>56322</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="B19" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>134</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="20" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+    <row r="20" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
         <v>56323</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C20" s="4" t="s">
+      <c r="B20" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>135</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="21" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+    <row r="21" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
         <v>56324</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="B21" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>136</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="22" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+    <row r="22" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
         <v>56325</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C22" s="4" t="s">
+      <c r="B22" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>137</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="23" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+    <row r="23" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
         <v>56326</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23" s="4" t="s">
+      <c r="B23" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>138</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="24" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+    <row r="24" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
         <v>56327</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C24" s="4" t="s">
+      <c r="B24" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>139</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="25" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+    <row r="25" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
         <v>56328</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="B25" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>140</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="26" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+    <row r="26" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
         <v>57403</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26" s="4" t="s">
+      <c r="B26" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>231</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="27" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+    <row r="27" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
         <v>56329</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" s="4" t="s">
+      <c r="B27" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>141</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="28" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
+    <row r="28" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
         <v>56330</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" s="4" t="s">
+      <c r="B28" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>142</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="29" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
+    <row r="29" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
         <v>56331</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="B29" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>143</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="30" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
+    <row r="30" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
         <v>56332</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C30" s="4" t="s">
+      <c r="B30" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="31" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
+    <row r="31" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
         <v>56333</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="B31" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>205</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="32" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
+    <row r="32" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
         <v>56334</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="4" t="s">
+      <c r="B32" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>145</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
+    <row r="33" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
         <v>56335</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C33" s="4" t="s">
+      <c r="B33" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>146</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
+    <row r="34" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
         <v>56336</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="4" t="s">
+      <c r="B34" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>147</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="35" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
+    <row r="35" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
         <v>56337</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C35" s="4" t="s">
+      <c r="B35" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>148</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="36" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
+    <row r="36" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
         <v>56338</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="4" t="s">
+      <c r="B36" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>149</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="37" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
+    <row r="37" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
         <v>56339</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C37" s="4" t="s">
+      <c r="B37" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>150</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
+    <row r="38" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
         <v>56340</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C38" s="4" t="s">
+      <c r="B38" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>129</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="39" spans="1:5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
+    <row r="39" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
         <v>56341</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C39" s="4" t="s">
+      <c r="B39" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>151</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="40" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
+    <row r="40" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
         <v>56342</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C40" s="4" t="s">
+      <c r="B40" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>152</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="1" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A41" s="6">
+      <c r="A41" s="1">
         <v>56061</v>
       </c>
-      <c r="B41" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C41" s="8" t="s">
+      <c r="B41" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D41" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="E41" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A42">
+    <row r="42" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
         <v>56124</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C42" s="4" t="s">
+      <c r="B42" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>153</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A43">
+    <row r="43" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
         <v>56175</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C43" s="4" t="s">
+      <c r="B43" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>154</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="44" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A44" s="6">
+    <row r="44" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
         <v>56126</v>
       </c>
-      <c r="B44" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C44" s="8" t="s">
+      <c r="B44" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E44" s="6" t="s">
+      <c r="E44" s="1" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A45" s="6">
+      <c r="A45" s="1">
         <v>56127</v>
       </c>
-      <c r="B45" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C45" s="8" t="s">
+      <c r="B45" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="D45" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="E45" s="6" t="s">
+      <c r="E45" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A46" s="6">
+      <c r="A46" s="1">
         <v>56378</v>
       </c>
-      <c r="B46" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C46" s="8" t="s">
+      <c r="B46" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D46" s="11" t="s">
+      <c r="D46" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="E46" s="6" t="s">
+      <c r="E46" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A47" s="6">
+      <c r="A47" s="1">
         <v>56379</v>
       </c>
-      <c r="B47" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C47" s="8" t="s">
+      <c r="B47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="E47" s="6" t="s">
+      <c r="E47" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="48" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A48">
+    <row r="48" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
         <v>56416</v>
       </c>
-      <c r="B48" t="s">
-        <v>76</v>
-      </c>
-      <c r="C48" s="4" t="s">
+      <c r="B48" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>155</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A49" s="6">
+      <c r="A49" s="1">
         <v>56417</v>
       </c>
-      <c r="B49" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C49" s="8" t="s">
+      <c r="B49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D49" s="11" t="s">
+      <c r="D49" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="E49" s="6" t="s">
+      <c r="E49" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A50" s="9">
+      <c r="A50" s="4">
         <v>56476</v>
       </c>
-      <c r="B50" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C50" s="8" t="s">
+      <c r="B50" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E50" s="6" t="s">
+      <c r="E50" s="1" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A51" s="9">
+      <c r="A51" s="4">
         <v>56477</v>
       </c>
-      <c r="B51" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C51" s="8" t="s">
+      <c r="B51" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E51" s="6" t="s">
+      <c r="E51" s="1" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A52" s="6">
+      <c r="A52" s="1">
         <v>56158</v>
       </c>
-      <c r="B52" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C52" s="8" t="s">
+      <c r="B52" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D52" s="11" t="s">
+      <c r="D52" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="E52" s="6" t="s">
+      <c r="E52" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A53" s="6">
+      <c r="A53" s="1">
         <v>56159</v>
       </c>
-      <c r="B53" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C53" s="8" t="s">
+      <c r="B53" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D53" s="11" t="s">
+      <c r="D53" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="E53" s="6" t="s">
+      <c r="E53" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A54" s="6">
+      <c r="A54" s="1">
         <v>56160</v>
       </c>
-      <c r="B54" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C54" s="8" t="s">
+      <c r="B54" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D54" s="14" t="s">
+      <c r="D54" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E54" s="6" t="s">
+      <c r="E54" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A55" s="6">
+      <c r="A55" s="1">
         <v>56161</v>
       </c>
-      <c r="B55" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C55" s="8" t="s">
+      <c r="B55" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D55" s="11" t="s">
+      <c r="D55" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="E55" s="6" t="s">
+      <c r="E55" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A56" s="6">
+      <c r="A56" s="1">
         <v>56162</v>
       </c>
-      <c r="B56" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C56" s="8" t="s">
+      <c r="B56" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D56" s="11" t="s">
+      <c r="D56" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E56" s="6" t="s">
+      <c r="E56" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A57" s="6">
+      <c r="A57" s="1">
         <v>56163</v>
       </c>
-      <c r="B57" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="D57" s="14" t="s">
+      <c r="B57" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D57" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E57" s="6" t="s">
+      <c r="E57" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="58" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A58" s="6">
+    <row r="58" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
         <v>56181</v>
       </c>
-      <c r="B58" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C58" s="8" t="s">
+      <c r="B58" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C58" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D58" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E58" s="6" t="s">
+      <c r="E58" s="1" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A59" s="6">
+      <c r="A59" s="1">
         <v>56164</v>
       </c>
-      <c r="B59" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C59" s="8" t="s">
+      <c r="B59" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C59" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D59" s="11" t="s">
+      <c r="D59" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="E59" s="6" t="s">
+      <c r="E59" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A60" s="6">
+      <c r="A60" s="1">
         <v>56165</v>
       </c>
-      <c r="B60" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C60" s="8" t="s">
+      <c r="B60" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C60" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D60" s="11" t="s">
+      <c r="D60" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="E60" s="6" t="s">
+      <c r="E60" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A61" s="6">
+      <c r="A61" s="1">
         <v>56457</v>
       </c>
-      <c r="B61" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C61" s="8" t="s">
+      <c r="B61" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E61" s="6" t="s">
+      <c r="E61" s="1" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A62" s="6">
+      <c r="A62" s="1">
         <v>56461</v>
       </c>
-      <c r="B62" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C62" s="8" t="s">
+      <c r="B62" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C62" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D62" s="11" t="s">
+      <c r="D62" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="E62" s="6" t="s">
+      <c r="E62" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A63" s="6">
+      <c r="A63" s="1">
         <v>56462</v>
       </c>
-      <c r="B63" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C63" s="8" t="s">
+      <c r="B63" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D63" s="11" t="s">
+      <c r="D63" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="E63" s="6" t="s">
+      <c r="E63" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="64" spans="1:5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A64" s="6">
+    <row r="64" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
         <v>56463</v>
       </c>
-      <c r="B64" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C64" s="4" t="s">
+      <c r="B64" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>158</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A65" s="6">
+      <c r="A65" s="1">
         <v>56464</v>
       </c>
-      <c r="B65" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C65" s="8" t="s">
+      <c r="B65" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D65" s="11" t="s">
+      <c r="D65" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="E65" s="6" t="s">
+      <c r="E65" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A66" s="6">
+      <c r="A66" s="1">
         <v>56465</v>
       </c>
-      <c r="B66" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C66" s="8" t="s">
+      <c r="B66" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="D66" s="11" t="s">
+      <c r="D66" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="E66" s="6" t="s">
+      <c r="E66" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A67" s="6">
+      <c r="A67" s="1">
         <v>56466</v>
       </c>
-      <c r="B67" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C67" s="8" t="s">
+      <c r="B67" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C67" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D67" s="7" t="s">
+      <c r="D67" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="E67" s="6" t="s">
+      <c r="E67" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A68" s="6">
+    <row r="68" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
         <v>56469</v>
       </c>
-      <c r="B68" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C68" s="4" t="s">
+      <c r="B68" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>159</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A69" s="6">
+      <c r="A69" s="1">
         <v>56467</v>
       </c>
-      <c r="B69" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C69" s="8" t="s">
+      <c r="B69" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D69" s="11" t="s">
+      <c r="D69" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="E69" s="10" t="s">
+      <c r="E69" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A70" s="6">
+      <c r="A70" s="1">
         <v>56468</v>
       </c>
-      <c r="B70" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C70" s="8" t="s">
+      <c r="B70" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="D70" s="7" t="s">
+      <c r="D70" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E70" s="6" t="s">
+      <c r="E70" s="1" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A71" s="6">
+      <c r="A71" s="1">
         <v>56170</v>
       </c>
-      <c r="B71" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C71" s="8" t="s">
+      <c r="B71" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C71" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D71" s="11" t="s">
+      <c r="D71" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="E71" s="6" t="s">
+      <c r="E71" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A72" s="6">
+      <c r="A72" s="1">
         <v>56171</v>
       </c>
-      <c r="B72" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C72" s="8" t="s">
+      <c r="B72" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C72" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D72" s="11" t="s">
+      <c r="D72" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="E72" s="6" t="s">
+      <c r="E72" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A73" s="6">
+      <c r="A73" s="1">
         <v>56172</v>
       </c>
-      <c r="B73" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C73" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="D73" s="14" t="s">
+      <c r="B73" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D73" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E73" s="6" t="s">
+      <c r="E73" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A74" s="6">
+      <c r="A74" s="1">
         <v>56173</v>
       </c>
-      <c r="B74" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C74" s="8" t="s">
+      <c r="B74" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C74" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D74" s="11" t="s">
+      <c r="D74" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="E74" s="6" t="s">
+      <c r="E74" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A75" s="6">
+      <c r="A75" s="1">
         <v>56174</v>
       </c>
-      <c r="B75" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C75" s="8" t="s">
+      <c r="B75" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C75" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D75" s="11" t="s">
+      <c r="D75" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E75" s="6" t="s">
+      <c r="E75" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A76" s="6">
+      <c r="A76" s="1">
         <v>56125</v>
       </c>
-      <c r="B76" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C76" s="8" t="s">
+      <c r="B76" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C76" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D76" s="14" t="s">
+      <c r="D76" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E76" s="10" t="s">
+      <c r="E76" s="5" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A77" s="6">
+      <c r="A77" s="1">
         <v>56182</v>
       </c>
-      <c r="B77" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C77" s="8" t="s">
+      <c r="B77" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C77" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D77" s="7" t="s">
+      <c r="D77" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E77" s="6" t="s">
+      <c r="E77" s="1" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A78" s="6">
+      <c r="A78" s="1">
         <v>56176</v>
       </c>
-      <c r="B78" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C78" s="8" t="s">
+      <c r="B78" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C78" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D78" s="11" t="s">
+      <c r="D78" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="E78" s="6" t="s">
+      <c r="E78" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A79" s="6">
+      <c r="A79" s="1">
         <v>56177</v>
       </c>
-      <c r="B79" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C79" s="8" t="s">
+      <c r="B79" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C79" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D79" s="11" t="s">
+      <c r="D79" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="E79" s="6" t="s">
+      <c r="E79" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A80" s="6">
+      <c r="A80" s="1">
         <v>56478</v>
       </c>
-      <c r="B80" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C80" s="8" t="s">
+      <c r="B80" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C80" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D80" s="11" t="s">
+      <c r="D80" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="E80" s="6" t="s">
+      <c r="E80" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A81" s="6">
+      <c r="A81" s="1">
         <v>56479</v>
       </c>
-      <c r="B81" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C81" s="8" t="s">
+      <c r="B81" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C81" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D81" s="14" t="s">
+      <c r="D81" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="E81" s="6" t="s">
+      <c r="E81" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A82" s="6">
+      <c r="A82" s="1">
         <v>56480</v>
       </c>
-      <c r="B82" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C82" s="8" t="s">
+      <c r="B82" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C82" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D82" s="14" t="s">
+      <c r="D82" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E82" s="6" t="s">
+      <c r="E82" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A83" s="6">
+      <c r="A83" s="1">
         <v>56482</v>
       </c>
-      <c r="B83" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C83" s="8" t="s">
+      <c r="B83" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C83" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D83" s="11" t="s">
+      <c r="D83" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="E83" s="6" t="s">
+      <c r="E83" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A84" s="6">
+      <c r="A84" s="1">
         <v>56481</v>
       </c>
-      <c r="B84" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C84" s="8" t="s">
+      <c r="B84" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C84" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D84" s="11" t="s">
+      <c r="D84" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="E84" s="6" t="s">
+      <c r="E84" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A85" s="6">
+      <c r="A85" s="1">
         <v>56492</v>
       </c>
-      <c r="B85" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C85" s="8" t="s">
+      <c r="B85" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C85" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D85" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="E85" s="6" t="s">
+      <c r="D85" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="E85" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A86" s="6">
+      <c r="A86" s="1">
         <v>56493</v>
       </c>
-      <c r="B86" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C86" s="8" t="s">
+      <c r="B86" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C86" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D86" s="14" t="s">
+      <c r="D86" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E86" s="6" t="s">
+      <c r="E86" s="1" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A87" s="6">
+      <c r="A87" s="1">
         <v>56496</v>
       </c>
-      <c r="B87" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C87" s="8" t="s">
+      <c r="B87" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C87" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D87" s="11" t="s">
+      <c r="D87" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="E87" s="6" t="s">
+      <c r="E87" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A88" s="6">
+      <c r="A88" s="1">
         <v>56186</v>
       </c>
-      <c r="B88" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C88" s="8" t="s">
+      <c r="B88" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C88" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D88" s="11" t="s">
+      <c r="D88" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="E88" s="6" t="s">
+      <c r="E88" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A89" s="6">
+      <c r="A89" s="1">
         <v>56187</v>
       </c>
-      <c r="B89" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C89" s="8" t="s">
+      <c r="B89" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C89" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D89" s="11" t="s">
+      <c r="D89" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="E89" s="6" t="s">
+      <c r="E89" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="90" spans="1:5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A90" s="6">
+    <row r="90" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
         <v>56188</v>
       </c>
-      <c r="B90" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C90" s="4" t="s">
+      <c r="B90" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C90" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D90" s="7" t="s">
+      <c r="D90" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E90" s="12" t="s">
+      <c r="E90" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A91" s="6">
+      <c r="A91" s="1">
         <v>56189</v>
       </c>
-      <c r="B91" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C91" s="8" t="s">
+      <c r="B91" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C91" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D91" s="11" t="s">
+      <c r="D91" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="E91" s="6" t="s">
+      <c r="E91" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="92" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A92" s="6">
+    <row r="92" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
         <v>56190</v>
       </c>
-      <c r="B92" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C92" s="4" t="s">
+      <c r="B92" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C92" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D92" s="7" t="s">
+      <c r="D92" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E92" s="6" t="s">
+      <c r="E92" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="93" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A93" s="6">
+    <row r="93" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
         <v>56191</v>
       </c>
-      <c r="B93" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C93" s="4" t="s">
+      <c r="B93" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C93" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D93" s="7" t="s">
+      <c r="D93" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E93" s="6" t="s">
+      <c r="E93" s="1" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A94" s="6">
+      <c r="A94" s="1">
         <v>56192</v>
       </c>
-      <c r="B94" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C94" s="8" t="s">
+      <c r="B94" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C94" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D94" s="11" t="s">
+      <c r="D94" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="E94" s="6" t="s">
+      <c r="E94" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A95" s="6">
+      <c r="A95" s="1">
         <v>56193</v>
       </c>
-      <c r="B95" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C95" s="8" t="s">
+      <c r="B95" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C95" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D95" s="11" t="s">
+      <c r="D95" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="E95" s="6" t="s">
+      <c r="E95" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A96" s="6">
+      <c r="A96" s="1">
         <v>56498</v>
       </c>
-      <c r="B96" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C96" s="8" t="s">
+      <c r="B96" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C96" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="D96" s="7" t="s">
+      <c r="D96" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E96" s="6" t="s">
+      <c r="E96" s="1" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A97" s="6">
+      <c r="A97" s="1">
         <v>56499</v>
       </c>
-      <c r="B97" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C97" s="8" t="s">
+      <c r="B97" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C97" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D97" s="11" t="s">
+      <c r="D97" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="E97" s="6" t="s">
+      <c r="E97" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A98" s="6">
+      <c r="A98" s="1">
         <v>56500</v>
       </c>
-      <c r="B98" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C98" s="8" t="s">
+      <c r="B98" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C98" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D98" s="14" t="s">
+      <c r="D98" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="E98" s="6" t="s">
+      <c r="E98" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A99" s="6">
+      <c r="A99" s="1">
         <v>56501</v>
       </c>
-      <c r="B99" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C99" s="8" t="s">
+      <c r="B99" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C99" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D99" s="14" t="s">
+      <c r="D99" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E99" s="6" t="s">
+      <c r="E99" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A100" s="6">
+      <c r="A100" s="1">
         <v>56503</v>
       </c>
-      <c r="B100" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C100" s="8" t="s">
+      <c r="B100" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C100" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D100" s="11" t="s">
+      <c r="D100" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="E100" s="6" t="s">
+      <c r="E100" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A101" s="6">
+      <c r="A101" s="1">
         <v>56506</v>
       </c>
-      <c r="B101" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C101" s="8" t="s">
+      <c r="B101" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C101" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="D101" s="11" t="s">
+      <c r="D101" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="E101" s="6" t="s">
+      <c r="E101" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A102" s="6">
+      <c r="A102" s="1">
         <v>56519</v>
       </c>
-      <c r="B102" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C102" s="8" t="s">
+      <c r="B102" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C102" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D102" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="E102" s="6" t="s">
+      <c r="D102" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="E102" s="1" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A103" s="6">
+      <c r="A103" s="1">
         <v>56520</v>
       </c>
-      <c r="B103" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C103" s="8" t="s">
+      <c r="B103" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C103" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D103" s="14" t="s">
+      <c r="D103" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E103" s="6" t="s">
+      <c r="E103" s="1" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A104" s="6">
+      <c r="A104" s="1">
         <v>56522</v>
       </c>
-      <c r="B104" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C104" s="8" t="s">
+      <c r="B104" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C104" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D104" s="11" t="s">
+      <c r="D104" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="E104" s="6" t="s">
+      <c r="E104" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="105" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A105" s="6">
+    <row r="105" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
         <v>56194</v>
       </c>
-      <c r="B105" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C105" s="8" t="s">
+      <c r="B105" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C105" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D105" s="7" t="s">
+      <c r="D105" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E105" s="6" t="s">
+      <c r="E105" s="1" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A106" s="6">
+      <c r="A106" s="1">
         <v>56523</v>
       </c>
-      <c r="B106" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C106" s="8" t="s">
+      <c r="B106" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C106" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D106" s="7" t="s">
+      <c r="D106" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E106" s="6" t="s">
+      <c r="E106" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="107" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A107">
+    <row r="107" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
         <v>56664</v>
       </c>
-      <c r="B107" t="s">
-        <v>76</v>
-      </c>
-      <c r="C107" s="8" t="s">
+      <c r="B107" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C107" s="3" t="s">
         <v>230</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E107" t="s">
+      <c r="E107" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="108" spans="1:5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A108">
+    <row r="108" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
         <v>56665</v>
       </c>
-      <c r="B108" t="s">
-        <v>76</v>
-      </c>
-      <c r="C108" s="8" t="s">
+      <c r="B108" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C108" s="3" t="s">
         <v>228</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="E108" t="s">
+      <c r="E108" s="1" t="s">
         <v>226</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualizacion de Datos en Archivos Excel
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - CREDIN - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - CREDIN - Escenarios y Casos de Pruebas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79AA4C1-E4C6-44DA-AAD4-97F8B2C467E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEAD3C2-98BE-4278-A628-A3B660C5CFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -822,16 +822,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">

</xml_diff>

<commit_message>
Acciones de refund, TCs de credito forzado, otros TCs de Sprint 40
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - CREDIN - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - CREDIN - Escenarios y Casos de Pruebas.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEAD3C2-98BE-4278-A628-A3B660C5CFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBF2375-79FE-487B-AC71-C501E852EDB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credin" sheetId="7" r:id="rId1"/>
+    <sheet name="CREDITO FORZADO" sheetId="9" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Credin!$A$1:$E$108</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'CREDITO FORZADO'!$A$1:$E$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="272">
   <si>
     <t>Parametros</t>
   </si>
@@ -757,6 +759,99 @@
   </si>
   <si>
     <t>"objeto":{"tipo":"TRANSFERENCIA"},"umbral_riesgo":100,"debito":{"cuit":"20000000222","banco":"000","sucursal":"SUC 207","cuenta":{"cbu":"0000207500000000000055"},"titular":"string"},"credito":{"cuit":"20263275064","banco":"000","sucursal":"0097","cuenta":{"cbu":"0000097000000000000116"},"titular":"string"},"concepto":"VAR","idUsuario":11231,"idComprobante":9228098,"importe":{"moneda":"032","importe":2950},"mismoTitular":0,"ori_trx":"","ori_terminal":"","ori_adicional":"","datosGenerador":{"ipCliente":"","tipoDispositivo":"","plataforma":"","imsi":"","imei":"","ubicacion":{"lat":0,"lng":0,"precision":0}},"descripcion":"Descripcion"</t>
+  </si>
+  <si>
+    <t>Credito*-&gt;aviso*</t>
+  </si>
+  <si>
+    <t>CashOut*-&gt;aviso*</t>
+  </si>
+  <si>
+    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con codigo 00: Credito realizado - Credin - OK</t>
+  </si>
+  <si>
+    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con codigo 00: Credito realizado - Cashout - OK</t>
+  </si>
+  <si>
+    <t>Credito Forzado - Agregado a broker/push -CVU-CVU- AvisoCredito responde un 200 con código 00: Credito realizado - Debin Spot- OK</t>
+  </si>
+  <si>
+    <t>Debin*-&gt;ConfirmaDebitoCVU*-&gt;ConfirmaDebito*-&gt;aviso*</t>
+  </si>
+  <si>
+    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con codigo 00: Credito realizado - Debin QR Coelsa Coelsa - OK</t>
+  </si>
+  <si>
+    <t>QRDebin*-&gt;ConfirmaDebito*-&gt;aviso*</t>
+  </si>
+  <si>
+    <t>Credito Forzado - Agregado a broker/push - DebinQR Coelsa Billetera - OK</t>
+  </si>
+  <si>
+    <t>Debin*-&gt;ConfirmaDebitoCVU*-&gt;ConfirmaDebito*-&gt;ContraCargo*-&gt;aviso*</t>
+  </si>
+  <si>
+    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con codigo 00: Credito realizado - Devolucion - OK</t>
+  </si>
+  <si>
+    <t>QRDebin*-&gt;ConfirmaDebito*-&gt;QRSolicitudContraCargo*-&gt;aviso*</t>
+  </si>
+  <si>
+    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con codigo 00: Credito realizado - Contracargo QR Coelsa Coelsa - OK</t>
+  </si>
+  <si>
+    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con codigo 00: Credito realizado - Refund QR Coelsa Billetera - OK</t>
+  </si>
+  <si>
+    <t>QRDebin*-&gt;ConfirmaDebito*-&gt;RefundValidation-&gt;Refund-&gt;aviso*</t>
+  </si>
+  <si>
+    <t>Credito Forzado - Agregado a broker/push -CVU-CVU- AvisoCredito responde un 200 con codigo 00: Credito realizado - Debin Recurrente - OK</t>
+  </si>
+  <si>
+    <t>Credito Forzado - Agregado a broker/push -CBU-CBU- AvisoCredito responde un 200 con codigo 00: Credito realizado - Debin Recurrente - OK</t>
+  </si>
+  <si>
+    <t>Debin*-&gt;ConfirmaDebito*-&gt;aviso*</t>
+  </si>
+  <si>
+    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con codigo 00: Credito realizado - TRX ISO - OK</t>
+  </si>
+  <si>
+    <t>"umbral_riesgo":100,"debito":{"cuit":"20000009998","banco":"998","sucursal":"0547","cuenta":{"cbu":"9980547400000000000055"},"titular":"string"},"credito":{"cuit":"23076812179","banco":"415","sucursal":"0999","cuenta":{"cbu":"4150999718001586640025"},"titular":"string"},"importe":{"importe":4500}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>"objeto":{"tipo":"CASHOUT"},"credito":{"cuit":"20956746117","banco":"000","sucursal":"0213","cuenta":{"cbu":"0000213699900070000000"},"titular":""},"debito":{"cuit":"20333048494","banco":"998","sucursal":"8851","cuenta":{"cbu":"9988851800000000000628"},"titular":"PRUEBAS COELSA CASHOUT"},"importe":{"importe":10}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>"operacion":{"detalle":{"importe":360}}}|"operacion":{"detalle":{"importe":360}}}|"operacion":{"detalle":{"importe":360}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>"operacion":{"detalle":{"importe":1000}}}|"operacion":{"detalle":{"importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>"operacion":{"detalle":{"importe":1000,"qr":"00020101021143160012com.todopago44110007com.agr48260012com.todopago010627571950150011309598932565204970053030325802AR5922Jordan Empresa Preprod6013VILLA URQUIZA6304d9da","id_billetera":4}}}|"operacion":{"comprador":{"cuit":"23000009989","cuenta":{"cbu":"9985340400000000000529"}},"detalle":{"ori_terminal":"","ori_adicional":"","moneda":"032","importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"recurrencia":true,"prestacion":"PrestacionAUT"},"detalle":{"importe":360}}}|"operacion":{"detalle":{"importe":360}}}|"operacion":{"detalle":{"importe":360}}}|"operacionOriginal":{"detalle":{"importe":360}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>"operacion":{"detalle":{"importe":1000}}}|"operacion":{"detalle":{"importe":1000}}}|"operacion_original":{"detalle":{"importe":250}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>"operacion":{"detalle":{"importe":1000,"qr":"00020101021143160012com.todopago44110007com.agr48260012com.todopago010627571950150011309598932565204970053030325802AR5922Jordan Empresa Preprod6013VILLA URQUIZA6304d9da","id_billetera":4}}}|"operacion":{"detalle":{"importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"recurrencia":true,"prestacion":"PrestacionAUT"},"detalle":{"importe":360}}}|"operacion":{"detalle":{"importe":360}}}|"operacion":{"detalle":{"importe":360}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20333048494","cbu":"9988851800000000000628","banco":"998","recurrencia":true,"prestacion":"PRESTACION23456"},"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420","alias":""}},"detalle":{"importe":199.02}}}|"operacion":{"comprador":{"cuit":"20000009963","cuenta":{"cbu":"9984788700000000000420"}},"detalle":{"importe":199.02}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>CreditoISO*-&gt;aviso*</t>
+  </si>
+  <si>
+    <t>"producto":"iso"|"id":"debin.id","aviso":"all","producto":"responder"</t>
   </si>
 </sst>
 </file>
@@ -778,12 +873,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -798,7 +905,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -817,6 +924,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1100,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63218BCB-F1F0-4D18-A551-3DB8181D382F}">
   <dimension ref="A1:E108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="D97" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2954,4 +3082,204 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6569509-97C1-4C00-933A-2630948AFC33}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="88.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="53.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="128.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
+        <v>62071</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <v>61223</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="D3" s="17"/>
+      <c r="E3" s="15" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>61234</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>61323</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>61435</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>61452</v>
+      </c>
+      <c r="B7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>61190</v>
+      </c>
+      <c r="B8" t="s">
+        <v>248</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>61525</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>61212</v>
+      </c>
+      <c r="B10" t="s">
+        <v>250</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>61201</v>
+      </c>
+      <c r="B11" t="s">
+        <v>252</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>61168</v>
+      </c>
+      <c r="B12" t="s">
+        <v>246</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Mas casos de Payment Validation
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - CREDIN - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - CREDIN - Escenarios y Casos de Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBF2375-79FE-487B-AC71-C501E852EDB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16A6C06-D150-46C4-9BAD-06668CCEE503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -905,7 +905,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -942,9 +942,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3088,14 +3085,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6569509-97C1-4C00-933A-2630948AFC33}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="67" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="88.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="53.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="128.140625" style="1" customWidth="1"/>
@@ -3135,48 +3132,48 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+      <c r="A3" s="12">
+        <v>61234</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="14" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>61323</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>61223</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B5" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C5" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="15" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="1" t="s">
         <v>244</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
-        <v>61234</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
-        <v>61323</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
payment, paymentvalidation y qrsolicitudcontracargo
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - CREDIN - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - CREDIN - Escenarios y Casos de Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FF28C8-CB28-42E2-839C-770F76F8CC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C29EA84-9454-4722-83A2-D299EE9AFC8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="868" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -873,13 +873,13 @@
     <t>"banco":"044","objeto":{},"credito":{"cuit":"20000000095","banco":"000","sucursal":"0000","cuenta":{"cbu":"0440000400000000000093"}},"debito":{"cuit":"'20000000095","banco":"044","sucursal":"0000","cuenta":{"cbu":"0440000400000000000109"}}}|"id":"debin.id","aviso":"all","producto":"CreditoHP"</t>
   </si>
   <si>
-    <t>"banco":"044","umbral_riesgo":100,"objeto":{},"credito":{"cuit":"20000000001","banco":"044","sucursal":"0000","cuenta":{"cbu":"0440000400000000000000"}},"debito":{"cuit":"20000000001","banco":"044","sucursal":"0000","cuenta":{"cbu":"0440000400000000000017"}}}</t>
-  </si>
-  <si>
     <t>"banco":"044","umbral_riesgo":100,"objeto":{"tipo":"TRANSFERENCIA"},"credito":{"cuit":"20000000001","banco":"044","sucursal":"0000","cuenta":{"cbu":"0440000400000000000079"}},"debito":{"cuit":"20000000001","banco":"044","sucursal":"0000","cuenta":{"cbu":"0440000400000000000086"}}}|"id":"debin.id","aviso":"all","endpoint":"Credito404","producto":"responder"</t>
   </si>
   <si>
     <t>"banco":"044","umbral_riesgo":100,"objeto":{"tipo":"TRANSFERENCIA"},"credito":{"cuit":"20000000095","banco":"044","sucursal":"0000","cuenta":{"cbu":"0440000400000000000093"}},"debito":{"cuit":"20000000095","banco":"044","sucursal":"0000","cuenta":{"cbu":"0440000400000000000109"}}}|"banco":"044","id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>"banco":"044","umbral_riesgo":100,"credito":{"cuit":"20000000001","banco":"044","sucursal":"0000","cuenta":{"cbu":"0440000400000000000000"}},"debito":{"cuit":"20000000001","banco":"044","sucursal":"0000","cuenta":{"cbu":"0440000400000000000017"}}}</t>
   </si>
 </sst>
 </file>
@@ -3428,7 +3428,7 @@
         <v>76</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="E2" t="s">
         <v>272</v>
@@ -3442,7 +3442,7 @@
         <v>241</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E3" t="s">
         <v>273</v>
@@ -3456,7 +3456,7 @@
         <v>241</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="12" t="s">

</xml_diff>

<commit_message>
Casos de Credito Forzado, test suites y test files
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - CREDIN - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - CREDIN - Escenarios y Casos de Pruebas.xlsx
@@ -8,23 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC3C0C9-2D8C-448B-9B97-F8ABB23892B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC1A785-ED00-4B1C-8FBB-4E4CE248AB32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credin" sheetId="7" r:id="rId1"/>
-    <sheet name="CREDITO FORZADO HP" sheetId="9" r:id="rId2"/>
-    <sheet name="CF - CASHOUT" sheetId="10" r:id="rId3"/>
-    <sheet name="CF - CREDIN" sheetId="11" r:id="rId4"/>
-    <sheet name="CF - RECURRENTE CBU" sheetId="12" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'CF - CASHOUT'!$A$1:$E$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'CF - CREDIN'!$A$1:$E$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'CF - RECURRENTE CBU'!$A$1:$E$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Credin!$A$1:$E$108</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'CREDITO FORZADO HP'!$A$1:$E$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="241">
   <si>
     <t>Parametros</t>
   </si>
@@ -765,165 +757,6 @@
   </si>
   <si>
     <t>"objeto":{"tipo":"TRANSFERENCIA"},"umbral_riesgo":100,"debito":{"cuit":"20000000222","banco":"000","sucursal":"SUC 207","cuenta":{"cbu":"0000207500000000000055"},"titular":"string"},"credito":{"cuit":"20263275064","banco":"000","sucursal":"0097","cuenta":{"cbu":"0000097000000000000116"},"titular":"string"},"concepto":"VAR","idUsuario":11231,"idComprobante":9228098,"importe":{"moneda":"032","importe":2950},"mismoTitular":0,"ori_trx":"","ori_terminal":"","ori_adicional":"","datosGenerador":{"ipCliente":"","tipoDispositivo":"","plataforma":"","imsi":"","imei":"","ubicacion":{"lat":0,"lng":0,"precision":0}},"descripcion":"Descripcion"</t>
-  </si>
-  <si>
-    <t>Credito*-&gt;aviso*</t>
-  </si>
-  <si>
-    <t>CashOut*-&gt;aviso*</t>
-  </si>
-  <si>
-    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con codigo 00: Credito realizado - Credin - OK</t>
-  </si>
-  <si>
-    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con codigo 00: Credito realizado - Cashout - OK</t>
-  </si>
-  <si>
-    <t>Credito Forzado - Agregado a broker/push -CVU-CVU- AvisoCredito responde un 200 con código 00: Credito realizado - Debin Spot- OK</t>
-  </si>
-  <si>
-    <t>Debin*-&gt;ConfirmaDebitoCVU*-&gt;ConfirmaDebito*-&gt;aviso*</t>
-  </si>
-  <si>
-    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con codigo 00: Credito realizado - Debin QR Coelsa Coelsa - OK</t>
-  </si>
-  <si>
-    <t>QRDebin*-&gt;ConfirmaDebito*-&gt;aviso*</t>
-  </si>
-  <si>
-    <t>Credito Forzado - Agregado a broker/push - DebinQR Coelsa Billetera - OK</t>
-  </si>
-  <si>
-    <t>Debin*-&gt;ConfirmaDebitoCVU*-&gt;ConfirmaDebito*-&gt;ContraCargo*-&gt;aviso*</t>
-  </si>
-  <si>
-    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con codigo 00: Credito realizado - Devolucion - OK</t>
-  </si>
-  <si>
-    <t>QRDebin*-&gt;ConfirmaDebito*-&gt;QRSolicitudContraCargo*-&gt;aviso*</t>
-  </si>
-  <si>
-    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con codigo 00: Credito realizado - Contracargo QR Coelsa Coelsa - OK</t>
-  </si>
-  <si>
-    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con codigo 00: Credito realizado - Refund QR Coelsa Billetera - OK</t>
-  </si>
-  <si>
-    <t>QRDebin*-&gt;ConfirmaDebito*-&gt;RefundValidation-&gt;Refund-&gt;aviso*</t>
-  </si>
-  <si>
-    <t>Credito Forzado - Agregado a broker/push -CVU-CVU- AvisoCredito responde un 200 con codigo 00: Credito realizado - Debin Recurrente - OK</t>
-  </si>
-  <si>
-    <t>Credito Forzado - Agregado a broker/push -CBU-CBU- AvisoCredito responde un 200 con codigo 00: Credito realizado - Debin Recurrente - OK</t>
-  </si>
-  <si>
-    <t>Debin*-&gt;ConfirmaDebito*-&gt;aviso*</t>
-  </si>
-  <si>
-    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con codigo 00: Credito realizado - TRX ISO - OK</t>
-  </si>
-  <si>
-    <t>"operacion":{"detalle":{"importe":360}}}|"operacion":{"detalle":{"importe":360}}}|"operacion":{"detalle":{"importe":360}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
-  </si>
-  <si>
-    <t>"operacion":{"detalle":{"importe":1000}}}|"operacion":{"detalle":{"importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
-  </si>
-  <si>
-    <t>"operacion":{"detalle":{"importe":1000,"qr":"00020101021143160012com.todopago44110007com.agr48260012com.todopago010627571950150011309598932565204970053030325802AR5922Jordan Empresa Preprod6013VILLA URQUIZA6304d9da","id_billetera":4}}}|"operacion":{"comprador":{"cuit":"23000009989","cuenta":{"cbu":"9985340400000000000529"}},"detalle":{"ori_terminal":"","ori_adicional":"","moneda":"032","importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
-  </si>
-  <si>
-    <t>"operacion":{"vendedor":{"recurrencia":true,"prestacion":"PrestacionAUT"},"detalle":{"importe":360}}}|"operacion":{"detalle":{"importe":360}}}|"operacion":{"detalle":{"importe":360}}}|"operacionOriginal":{"detalle":{"importe":360}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
-  </si>
-  <si>
-    <t>"operacion":{"detalle":{"importe":1000}}}|"operacion":{"detalle":{"importe":1000}}}|"operacion_original":{"detalle":{"importe":250}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
-  </si>
-  <si>
-    <t>"operacion":{"detalle":{"importe":1000,"qr":"00020101021143160012com.todopago44110007com.agr48260012com.todopago010627571950150011309598932565204970053030325802AR5922Jordan Empresa Preprod6013VILLA URQUIZA6304d9da","id_billetera":4}}}|"operacion":{"detalle":{"importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
-  </si>
-  <si>
-    <t>"operacion":{"vendedor":{"recurrencia":true,"prestacion":"PrestacionAUT"},"detalle":{"importe":360}}}|"operacion":{"detalle":{"importe":360}}}|"operacion":{"detalle":{"importe":360}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
-  </si>
-  <si>
-    <t>CreditoISO*-&gt;aviso*</t>
-  </si>
-  <si>
-    <t>"producto":"iso"|"id":"debin.id","aviso":"all","producto":"responder"</t>
-  </si>
-  <si>
-    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde 403 - Cashout - OK</t>
-  </si>
-  <si>
-    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde 404 - Cashout - OK</t>
-  </si>
-  <si>
-    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde 403 - Credin - OK</t>
-  </si>
-  <si>
-    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde 404 - Credin - OK</t>
-  </si>
-  <si>
-    <t>Crédito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con código 07: Acreditación pendiente (EN SCREENING) - Credin - OK</t>
-  </si>
-  <si>
-    <t>Crédito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con código 02: Datos incorrectos - Credin - OK</t>
-  </si>
-  <si>
-    <t>Crédito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con código 05: Error interno - Credin - OK</t>
-  </si>
-  <si>
-    <t>|"id":"debin.id","aviso":"all","endpoint":"Credito403","producto":"responder"</t>
-  </si>
-  <si>
-    <t>|"id":"debin.id","aviso":"all","endpoint":"Credito404","producto":"responder"</t>
-  </si>
-  <si>
-    <t>|"id":"debin.id","aviso":"all","endpoint":"Codigo02","producto":"responder"</t>
-  </si>
-  <si>
-    <t>|"id":"debin.id","aviso":"all","endpoint":"Codigo07","producto":"responder"</t>
-  </si>
-  <si>
-    <t>|"id":"debin.id","aviso":"all","endpoint":"Codigo05","producto":"responder"</t>
-  </si>
-  <si>
-    <t>Credito Forzado - Agregado a broker/push -CBU-CBU - AvisoCredito responde 403 - Debin Recurrente - OK</t>
-  </si>
-  <si>
-    <t>Credito Forzado - Agregado a broker/push - CBU-CBU- AvisoCredito responde 404 - Debin Recurrente - OK</t>
-  </si>
-  <si>
-    <t>Crédito Forzado - Agregado a broker/push -CBU-CBU- AvisoCredito responde un 200 con código 07: Acreditación pendiente (EN SCREENING) - Debin Recurrente - OK</t>
-  </si>
-  <si>
-    <t>Crédito Forzado - Agregado a broker/push -CBU-CBU- AvisoCredito responde un 200 con código 02: Datos incorrectos - Debin Recurrente - OK</t>
-  </si>
-  <si>
-    <t>Crédito Forzado - Agregado a broker/push -CBU-CBU- AvisoCredito responde un 200 con código 05: Error interno - Debin Recurrente - OK</t>
-  </si>
-  <si>
-    <t>"banco":"044","credito":{"cuit":"20000000001","banco":"044","sucursal":"0000","cuenta":{"cbu":"0440000400000000000000"}},"debito":{"cuit":"20000000001","banco":"044","sucursal":"0000","cuenta":{"cbu":"0440000400000000000017"}}}|"id":"debin.id","aviso":"all","endpoint":"Credito403","producto":"responder"</t>
-  </si>
-  <si>
-    <t>"banco":"044","credito":{"cuit":"20000000001","banco":"044","sucursal":"0000","cuenta":{"cbu":"0440000400000000000079"}},"debito":{"cuit":"20000000001","banco":"044","sucursal":"0000","cuenta":{"cbu":"0440000400000000000086"}}}|"id":"debin.id","aviso":"all","endpoint":"Credito404","producto":"responder"</t>
-  </si>
-  <si>
-    <t>"banco":"044","credito":{"cuit":"20000000095","banco":"044","sucursal":"0000","cuenta":{"cbu":"0440000400000000000093"}},"debito":{"cuit":"20000000095","banco":"044","sucursal":"0000","cuenta":{"cbu":"0440000400000000000109"}}}|"id":"debin.id","aviso":"all","endpoint":"CreditoHP","producto":"responder"</t>
-  </si>
-  <si>
-    <t>"banco":"044","credito":{"cuit":"20000000001","banco":"044","sucursal":"0000","cuenta":{"cbu":"0440000400000000000147"}},"debito":{"cuit":"20000000001","banco":"044","sucursal":"0000","cuenta":{"cbu":"0440000400000000000154"}}}|"id":"debin.id","aviso":"all","endpoint":"Codigo07","producto":"responder"</t>
-  </si>
-  <si>
-    <t>"banco":"044","credito":{"cuit":"20000000001","banco":"044","sucursal":"0000","cuenta":{"cbu":"0440000400000000000161"}},"debito":{"cuit":"20000000001","banco":"044","sucursal":"0000","cuenta":{"cbu":"0440000400000000000178"}}}|"id":"debin.id","aviso":"all","endpoint":"Codigo02","producto":"responder"</t>
-  </si>
-  <si>
-    <t>"banco":"044","credito":{"cuit":"20000000001","banco":"044","sucursal":"0000","cuenta":{"cbu":"0440000400000000000192"}},"debito":{"cuit":"20000000001","banco":"044","sucursal":"0000","cuenta":{"cbu":"0440000400000000000208"}}}|"id":"debin.id","aviso":"all","endpoint":"Codigo05","producto":"responder"</t>
-  </si>
-  <si>
-    <t>"banco":"044","credito":{"cuit":"20000000001","banco":"044","sucursal":"0000","cuenta":{"cbu":"0440000400000000000123"}},"debito":{"cuit":"20000000001","banco":"044","sucursal":"0000","cuenta":{"cbu":"0440000400000000000130"}}}|"id":"debin.id","aviso":"all","endpoint":"Credito403","producto":"responder"</t>
-  </si>
-  <si>
-    <t>"banco":"044","operacion":{"vendedor":{"cuit":"20000000095","cbu":"0440000400000000000093","banco":"044","recurrencia":true,"prestacion":"Prestacion1"},"comprador":{"cuit":"20000000095","cuenta":{"cbu":"0440000400000000000109"}},"detalle":{"importe":199.02}}}|"banco":"044","operacion":{"comprador":{"cuit":"20000000095","cuenta":{"cbu":"0440000400000000000109"}},"detalle":{"importe":199.02}}}|"id":"debin.id","aviso":"all","endpoint":"CreditoHP","producto":"responder"</t>
   </si>
 </sst>
 </file>
@@ -945,24 +778,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -977,7 +798,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -996,24 +817,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1297,7 +1100,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63218BCB-F1F0-4D18-A551-3DB8181D382F}">
   <dimension ref="A1:E108"/>
   <sheetViews>
-    <sheetView topLeftCell="C34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -3151,501 +2954,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6569509-97C1-4C00-933A-2630948AFC33}">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="67" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="88.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="53.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="128.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
-        <v>62071</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>61435</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>61452</v>
-      </c>
-      <c r="B5" t="s">
-        <v>246</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>61190</v>
-      </c>
-      <c r="B6" t="s">
-        <v>248</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>261</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>61525</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>61212</v>
-      </c>
-      <c r="B8" t="s">
-        <v>250</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>61201</v>
-      </c>
-      <c r="B9" t="s">
-        <v>252</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>61168</v>
-      </c>
-      <c r="B10" t="s">
-        <v>246</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC0A671-2C0C-430F-865C-9634A4BA3E48}">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="88.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="128.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>61220</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
-        <v>61221</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>292</v>
-      </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>61223</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>292</v>
-      </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C34BCF1-B5AA-49E0-9E04-B6FDE423A4FE}">
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33" style="1" customWidth="1"/>
-    <col min="3" max="3" width="88.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="53.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="128.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>61231</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="14" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>61232</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="14" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>61234</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="14" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>61235</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>61239</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>61240</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>275</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4808394F-3102-4283-ADEC-8374D1FD01FB}">
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="67" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="88.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="53.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="128.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>61320</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="14" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>61321</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="14" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>61323</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>293</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>61324</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>61328</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>61329</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>285</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Validacion de tipo de contracargo y contracargoqr
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - CREDIN - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - CREDIN - Escenarios y Casos de Pruebas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA93AF68-8EFE-4D23-8716-B506D838824A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E8741D-0BBA-41E6-BC61-882D726DA7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credin" sheetId="7" r:id="rId1"/>
@@ -807,34 +807,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1121,1849 +1117,1848 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="88.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="53.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="89.7109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" customWidth="1"/>
+    <col min="3" max="3" width="88.26953125" customWidth="1"/>
+    <col min="4" max="4" width="53.81640625" customWidth="1"/>
+    <col min="5" max="5" width="89.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A2">
         <v>53630</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+    <row r="3" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>53631</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+    <row r="4" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>53632</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+    <row r="5" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A5">
         <v>53635</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+    <row r="6" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A6">
         <v>53636</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="7" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A7">
         <v>56124</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="12" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+    <row r="8" spans="1:5" s="6" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="6">
         <v>56476</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="10" t="s">
+      <c r="B8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="9" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A9">
         <v>56159</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="10" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A10">
         <v>56160</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="11" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A11">
         <v>56161</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="12" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A12">
         <v>56162</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="13" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A13">
         <v>56163</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+    <row r="14" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A14">
         <v>56181</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+    <row r="15" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A15">
         <v>56463</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+    <row r="16" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A16">
         <v>56172</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+    <row r="17" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A17">
         <v>56174</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+    <row r="18" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A18">
         <v>56480</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+    <row r="19" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A19">
         <v>56188</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="B19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+    <row r="20" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A20">
         <v>56501</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+    <row r="21" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A21">
         <v>53628</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="B21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+    <row r="22" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A22">
         <v>53629</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+    <row r="23" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A23">
         <v>53633</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+    <row r="24" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A24">
         <v>53634</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="B24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+    <row r="25" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A25">
         <v>53637</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+    <row r="26" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+      <c r="A26">
         <v>53638</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="3" t="s">
+      <c r="B26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+    <row r="27" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A27">
         <v>53639</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="3" t="s">
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+    <row r="28" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A28">
         <v>53640</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+    <row r="29" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A29">
         <v>53431</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="3" t="s">
+      <c r="B29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+    <row r="30" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A30">
         <v>53432</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" s="3" t="s">
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+    <row r="31" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A31">
         <v>53433</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31" s="3" t="s">
+      <c r="B31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+    <row r="32" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A32">
         <v>53434</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" s="3" t="s">
+      <c r="B32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+    <row r="33" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A33">
         <v>56322</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" s="3" t="s">
+      <c r="B33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+    <row r="34" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A34">
         <v>56323</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="B34" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+    <row r="35" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A35">
         <v>56324</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="3" t="s">
+      <c r="B35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+    <row r="36" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A36">
         <v>56325</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C36" s="3" t="s">
+      <c r="B36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
+    <row r="37" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A37">
         <v>56326</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C37" s="3" t="s">
+      <c r="B37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+    <row r="38" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A38">
         <v>56327</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" s="3" t="s">
+      <c r="B38" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
+    <row r="39" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A39">
         <v>56328</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C39" s="3" t="s">
+      <c r="B39" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
+    <row r="40" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A40">
         <v>57403</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C40" s="3" t="s">
+      <c r="B40" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
+    <row r="41" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A41">
         <v>56329</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C41" s="3" t="s">
+      <c r="B41" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
+    <row r="42" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A42">
         <v>56330</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C42" s="3" t="s">
+      <c r="B42" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
+    <row r="43" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A43">
         <v>56331</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C43" s="3" t="s">
+      <c r="B43" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
+    <row r="44" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A44">
         <v>56332</v>
       </c>
-      <c r="B44" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C44" s="3" t="s">
+      <c r="B44" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
+    <row r="45" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A45">
         <v>56333</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C45" s="3" t="s">
+      <c r="B45" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
+    <row r="46" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A46">
         <v>56334</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C46" s="3" t="s">
+      <c r="B46" t="s">
+        <v>56</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
+    <row r="47" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A47">
         <v>56335</v>
       </c>
-      <c r="B47" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C47" s="3" t="s">
+      <c r="B47" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
+    <row r="48" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A48">
         <v>56336</v>
       </c>
-      <c r="B48" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C48" s="3" t="s">
+      <c r="B48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D48" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A49" s="4">
+    <row r="49" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A49">
         <v>56337</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C49" s="3" t="s">
+      <c r="B49" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D49" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
+    <row r="50" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A50">
         <v>56338</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C50" s="3" t="s">
+      <c r="B50" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D50" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
+    <row r="51" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A51">
         <v>56339</v>
       </c>
-      <c r="B51" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C51" s="3" t="s">
+      <c r="B51" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D51" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A52" s="4">
+    <row r="52" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A52">
         <v>56340</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C52" s="3" t="s">
+      <c r="B52" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D52" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E52" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A53" s="4">
+    <row r="53" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+      <c r="A53">
         <v>56341</v>
       </c>
-      <c r="B53" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C53" s="3" t="s">
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D53" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E53" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
+    <row r="54" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A54">
         <v>56342</v>
       </c>
-      <c r="B54" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C54" s="3" t="s">
+      <c r="B54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D54" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="E54" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
+    <row r="55" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A55">
         <v>56061</v>
       </c>
-      <c r="B55" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C55" s="3" t="s">
+      <c r="B55" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="D55" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="E55" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
+    <row r="56" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A56">
         <v>56175</v>
       </c>
-      <c r="B56" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C56" s="3" t="s">
+      <c r="B56" t="s">
+        <v>56</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D56" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E56" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
+    <row r="57" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A57">
         <v>56126</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C57" s="3" t="s">
+      <c r="B57" t="s">
+        <v>56</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D57" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="E57" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
+    <row r="58" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A58">
         <v>56127</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C58" s="3" t="s">
+      <c r="B58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D58" s="6" t="s">
+      <c r="D58" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E58" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
+    <row r="59" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A59">
         <v>56378</v>
       </c>
-      <c r="B59" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C59" s="3" t="s">
+      <c r="B59" t="s">
+        <v>56</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D59" s="6" t="s">
+      <c r="D59" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="E59" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
+    <row r="60" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A60">
         <v>56379</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C60" s="3" t="s">
+      <c r="B60" t="s">
+        <v>56</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D60" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="E60" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
+    <row r="61" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A61">
         <v>56416</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C61" s="3" t="s">
+      <c r="B61" t="s">
+        <v>56</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="D61" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E61" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
+    <row r="62" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A62">
         <v>56417</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C62" s="3" t="s">
+      <c r="B62" t="s">
+        <v>56</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D62" s="6" t="s">
+      <c r="D62" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="E62" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A63" s="4">
+    <row r="63" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A63">
         <v>56477</v>
       </c>
-      <c r="B63" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C63" s="3" t="s">
+      <c r="B63" t="s">
+        <v>56</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="D63" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="E63" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
+    <row r="64" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A64">
         <v>56158</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C64" s="3" t="s">
+      <c r="B64" t="s">
+        <v>56</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D64" s="6" t="s">
+      <c r="D64" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="E64" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
+    <row r="65" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A65">
         <v>56164</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C65" s="3" t="s">
+      <c r="B65" t="s">
+        <v>56</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D65" s="6" t="s">
+      <c r="D65" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="E65" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
+    <row r="66" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A66">
         <v>56165</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C66" s="3" t="s">
+      <c r="B66" t="s">
+        <v>56</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D66" s="6" t="s">
+      <c r="D66" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E66" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
+    <row r="67" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A67">
         <v>56457</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C67" s="3" t="s">
+      <c r="B67" t="s">
+        <v>56</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D67" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E67" s="1" t="s">
+      <c r="E67" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
+    <row r="68" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+      <c r="A68">
         <v>56461</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C68" s="3" t="s">
+      <c r="B68" t="s">
+        <v>56</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D68" s="6" t="s">
+      <c r="D68" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="E68" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
+    <row r="69" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A69">
         <v>56462</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C69" s="3" t="s">
+      <c r="B69" t="s">
+        <v>56</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D69" s="6" t="s">
+      <c r="D69" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="E69" s="1" t="s">
+      <c r="E69" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
+    <row r="70" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A70">
         <v>56464</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C70" s="3" t="s">
+      <c r="B70" t="s">
+        <v>56</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D70" s="6" t="s">
+      <c r="D70" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="E70" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
+    <row r="71" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A71">
         <v>56465</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C71" s="3" t="s">
+      <c r="B71" t="s">
+        <v>56</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D71" s="6" t="s">
+      <c r="D71" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="E71" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
+    <row r="72" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A72">
         <v>56466</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C72" s="3" t="s">
+      <c r="B72" t="s">
+        <v>56</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="D72" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="E72" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
+    <row r="73" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A73">
         <v>56469</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C73" s="3" t="s">
+      <c r="B73" t="s">
+        <v>56</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D73" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="E73" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
+    <row r="74" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A74">
         <v>56467</v>
       </c>
-      <c r="B74" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C74" s="3" t="s">
+      <c r="B74" t="s">
+        <v>56</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D74" s="6" t="s">
+      <c r="D74" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="E74" s="5" t="s">
+      <c r="E74" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
+    <row r="75" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A75">
         <v>56468</v>
       </c>
-      <c r="B75" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C75" s="3" t="s">
+      <c r="B75" t="s">
+        <v>56</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="D75" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="E75" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
+    <row r="76" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A76">
         <v>56170</v>
       </c>
-      <c r="B76" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C76" s="3" t="s">
+      <c r="B76" t="s">
+        <v>56</v>
+      </c>
+      <c r="C76" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D76" s="6" t="s">
+      <c r="D76" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="E76" s="1" t="s">
+      <c r="E76" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
+    <row r="77" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A77">
         <v>56171</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C77" s="3" t="s">
+      <c r="B77" t="s">
+        <v>56</v>
+      </c>
+      <c r="C77" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D77" s="6" t="s">
+      <c r="D77" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="E77" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
+    <row r="78" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A78">
         <v>56173</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C78" s="3" t="s">
+      <c r="B78" t="s">
+        <v>56</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D78" s="6" t="s">
+      <c r="D78" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="E78" s="1" t="s">
+      <c r="E78" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
+    <row r="79" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A79">
         <v>56125</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C79" s="3" t="s">
+      <c r="B79" t="s">
+        <v>56</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D79" s="6" t="s">
+      <c r="D79" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E79" s="5" t="s">
+      <c r="E79" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
+    <row r="80" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A80">
         <v>56182</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C80" s="3" t="s">
+      <c r="B80" t="s">
+        <v>56</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="D80" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E80" s="1" t="s">
+      <c r="E80" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
+    <row r="81" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A81">
         <v>56176</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C81" s="3" t="s">
+      <c r="B81" t="s">
+        <v>56</v>
+      </c>
+      <c r="C81" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D81" s="6" t="s">
+      <c r="D81" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="E81" s="1" t="s">
+      <c r="E81" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
+    <row r="82" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A82">
         <v>56177</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C82" s="3" t="s">
+      <c r="B82" t="s">
+        <v>56</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D82" s="6" t="s">
+      <c r="D82" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="E82" s="1" t="s">
+      <c r="E82" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
+    <row r="83" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+      <c r="A83">
         <v>56478</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C83" s="3" t="s">
+      <c r="B83" t="s">
+        <v>56</v>
+      </c>
+      <c r="C83" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D83" s="6" t="s">
+      <c r="D83" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="E83" s="1" t="s">
+      <c r="E83" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
+    <row r="84" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+      <c r="A84">
         <v>56479</v>
       </c>
-      <c r="B84" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C84" s="3" t="s">
+      <c r="B84" t="s">
+        <v>56</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D84" s="6" t="s">
+      <c r="D84" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="E84" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
+    <row r="85" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A85">
         <v>56482</v>
       </c>
-      <c r="B85" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C85" s="3" t="s">
+      <c r="B85" t="s">
+        <v>56</v>
+      </c>
+      <c r="C85" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D85" s="6" t="s">
+      <c r="D85" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="E85" s="1" t="s">
+      <c r="E85" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
+    <row r="86" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A86">
         <v>56481</v>
       </c>
-      <c r="B86" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C86" s="3" t="s">
+      <c r="B86" t="s">
+        <v>56</v>
+      </c>
+      <c r="C86" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D86" s="6" t="s">
+      <c r="D86" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="E86" s="1" t="s">
+      <c r="E86" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
+    <row r="87" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A87">
         <v>56492</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C87" s="3" t="s">
+      <c r="B87" t="s">
+        <v>56</v>
+      </c>
+      <c r="C87" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D87" s="6" t="s">
+      <c r="D87" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="E87" s="1" t="s">
+      <c r="E87" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
+    <row r="88" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A88">
         <v>56493</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C88" s="3" t="s">
+      <c r="B88" t="s">
+        <v>56</v>
+      </c>
+      <c r="C88" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D88" s="6" t="s">
+      <c r="D88" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="E88" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
+    <row r="89" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A89">
         <v>56496</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C89" s="3" t="s">
+      <c r="B89" t="s">
+        <v>56</v>
+      </c>
+      <c r="C89" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D89" s="6" t="s">
+      <c r="D89" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="E89" s="1" t="s">
+      <c r="E89" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
+    <row r="90" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A90">
         <v>56186</v>
       </c>
-      <c r="B90" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C90" s="3" t="s">
+      <c r="B90" t="s">
+        <v>56</v>
+      </c>
+      <c r="C90" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D90" s="6" t="s">
+      <c r="D90" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="E90" s="1" t="s">
+      <c r="E90" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
+    <row r="91" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+      <c r="A91">
         <v>56187</v>
       </c>
-      <c r="B91" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C91" s="3" t="s">
+      <c r="B91" t="s">
+        <v>56</v>
+      </c>
+      <c r="C91" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D91" s="6" t="s">
+      <c r="D91" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="E91" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
+    <row r="92" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A92">
         <v>56189</v>
       </c>
-      <c r="B92" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C92" s="3" t="s">
+      <c r="B92" t="s">
+        <v>56</v>
+      </c>
+      <c r="C92" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D92" s="6" t="s">
+      <c r="D92" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="E92" s="1" t="s">
+      <c r="E92" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A93" s="1">
+    <row r="93" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A93">
         <v>56190</v>
       </c>
-      <c r="B93" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C93" s="3" t="s">
+      <c r="B93" t="s">
+        <v>56</v>
+      </c>
+      <c r="C93" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D93" s="2" t="s">
+      <c r="D93" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E93" s="1" t="s">
+      <c r="E93" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
+    <row r="94" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A94">
         <v>56191</v>
       </c>
-      <c r="B94" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C94" s="3" t="s">
+      <c r="B94" t="s">
+        <v>56</v>
+      </c>
+      <c r="C94" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D94" s="2" t="s">
+      <c r="D94" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E94" s="1" t="s">
+      <c r="E94" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
+    <row r="95" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A95">
         <v>56192</v>
       </c>
-      <c r="B95" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C95" s="3" t="s">
+      <c r="B95" t="s">
+        <v>56</v>
+      </c>
+      <c r="C95" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D95" s="6" t="s">
+      <c r="D95" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="E95" s="1" t="s">
+      <c r="E95" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
+    <row r="96" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A96">
         <v>56193</v>
       </c>
-      <c r="B96" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C96" s="3" t="s">
+      <c r="B96" t="s">
+        <v>56</v>
+      </c>
+      <c r="C96" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D96" s="6" t="s">
+      <c r="D96" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="E96" s="1" t="s">
+      <c r="E96" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
+    <row r="97" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A97">
         <v>56498</v>
       </c>
-      <c r="B97" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C97" s="3" t="s">
+      <c r="B97" t="s">
+        <v>56</v>
+      </c>
+      <c r="C97" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D97" s="2" t="s">
+      <c r="D97" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E97" s="1" t="s">
+      <c r="E97" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
+    <row r="98" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A98">
         <v>56499</v>
       </c>
-      <c r="B98" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C98" s="3" t="s">
+      <c r="B98" t="s">
+        <v>56</v>
+      </c>
+      <c r="C98" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D98" s="6" t="s">
+      <c r="D98" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="E98" s="1" t="s">
+      <c r="E98" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
+    <row r="99" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+      <c r="A99">
         <v>56500</v>
       </c>
-      <c r="B99" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C99" s="3" t="s">
+      <c r="B99" t="s">
+        <v>56</v>
+      </c>
+      <c r="C99" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D99" s="6" t="s">
+      <c r="D99" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="E99" s="1" t="s">
+      <c r="E99" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
+    <row r="100" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A100">
         <v>56503</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C100" s="3" t="s">
+      <c r="B100" t="s">
+        <v>56</v>
+      </c>
+      <c r="C100" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D100" s="6" t="s">
+      <c r="D100" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="E100" s="1" t="s">
+      <c r="E100" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
+    <row r="101" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A101">
         <v>56506</v>
       </c>
-      <c r="B101" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C101" s="3" t="s">
+      <c r="B101" t="s">
+        <v>56</v>
+      </c>
+      <c r="C101" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="D101" s="6" t="s">
+      <c r="D101" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="E101" s="1" t="s">
+      <c r="E101" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A102" s="1">
+    <row r="102" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A102">
         <v>56519</v>
       </c>
-      <c r="B102" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C102" s="3" t="s">
+      <c r="B102" t="s">
+        <v>56</v>
+      </c>
+      <c r="C102" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D102" s="6" t="s">
+      <c r="D102" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="E102" s="1" t="s">
+      <c r="E102" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
+    <row r="103" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A103">
         <v>56520</v>
       </c>
-      <c r="B103" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C103" s="3" t="s">
+      <c r="B103" t="s">
+        <v>56</v>
+      </c>
+      <c r="C103" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D103" s="6" t="s">
+      <c r="D103" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E103" s="1" t="s">
+      <c r="E103" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A104" s="1">
+    <row r="104" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A104">
         <v>56522</v>
       </c>
-      <c r="B104" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C104" s="3" t="s">
+      <c r="B104" t="s">
+        <v>56</v>
+      </c>
+      <c r="C104" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D104" s="6" t="s">
+      <c r="D104" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="E104" s="1" t="s">
+      <c r="E104" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A105" s="1">
+    <row r="105" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A105">
         <v>56194</v>
       </c>
-      <c r="B105" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C105" s="3" t="s">
+      <c r="B105" t="s">
+        <v>56</v>
+      </c>
+      <c r="C105" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D105" s="2" t="s">
+      <c r="D105" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E105" s="1" t="s">
+      <c r="E105" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A106" s="1">
+    <row r="106" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A106">
         <v>56523</v>
       </c>
-      <c r="B106" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C106" s="3" t="s">
+      <c r="B106" t="s">
+        <v>56</v>
+      </c>
+      <c r="C106" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D106" s="2" t="s">
+      <c r="D106" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E106" s="1" t="s">
+      <c r="E106" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A107" s="1">
+    <row r="107" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A107">
         <v>56664</v>
       </c>
-      <c r="B107" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C107" s="3" t="s">
+      <c r="B107" t="s">
+        <v>56</v>
+      </c>
+      <c r="C107" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="D107" s="2" t="s">
+      <c r="D107" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="E107" s="1" t="s">
+      <c r="E107" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A108" s="1">
+    <row r="108" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A108">
         <v>56665</v>
       </c>
-      <c r="B108" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C108" s="3" t="s">
+      <c r="B108" t="s">
+        <v>56</v>
+      </c>
+      <c r="C108" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D108" s="2" t="s">
+      <c r="D108" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="E108" s="1" t="s">
+      <c r="E108" t="s">
         <v>192</v>
       </c>
     </row>

</xml_diff>